<commit_message>
Generate Species from Specimens aggregation
</commit_message>
<xml_diff>
--- a/uploads/0BwPshgd2tnbbU0diUmgzVFhjS28.xlsx
+++ b/uploads/0BwPshgd2tnbbU0diUmgzVFhjS28.xlsx
@@ -500,15 +500,7 @@
         <color indexed="8"/>
         <rFont val="Helv"/>
       </rPr>
-      <t>bibliographicCitation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">bibliographicCitation </t>
     </r>
   </si>
   <si>
@@ -996,7 +988,7 @@
     <t>equinolofada</t>
   </si>
   <si>
-    <t>DIÂMETRO Min:13,79; Max:17,08; Med:15,24; DVPAD:0,79</t>
+    <t>Min:13,79; Max:17,08; Med:15,24; DVPAD:0,79</t>
   </si>
   <si>
     <t>Min:1,68; Max:1,97; Med:1,82; DVPAD:0,10</t>
@@ -1441,7 +1433,7 @@
     <t>Min:1,12; Max:1,39; Med:1,22; DVPAD:0,07</t>
   </si>
   <si>
-    <t>Min:38,33 Max:46,08; Med:42,53; DVPAD:1,86</t>
+    <t>Min:38,33; Max:46,08; Med:42,53; DVPAD:1,86</t>
   </si>
   <si>
     <t>Min:32,86; Max:38,48; Med:34,78; DVPAD:1,67</t>
@@ -2003,7 +1995,7 @@
     <t>suboblato a subprolato</t>
   </si>
   <si>
-    <t>DIÂMETRO Min:63,31; Max:75,58; Med:70,59; DVPAD:3,56</t>
+    <t>Min:63,31; Max:75,58; Med:70,59; DVPAD:3,56</t>
   </si>
   <si>
     <t>Min:0,58; Max:0,92; Med:0,84; DVPAD:0,10</t>
@@ -2056,10 +2048,10 @@
     <t>monossulcado</t>
   </si>
   <si>
-    <t>DIÂMETRO MENOR Min:51,80; Max:67,50; Med:60,28; DVPAD:3,99</t>
-  </si>
-  <si>
-    <t>DIÂMETRO MAIOR Min:57,12; Max:66,77; Med:60,45; DVPAD:2,80</t>
+    <t>Min:51,80; Max:67,50; Med:60,28; DVPAD:3,99</t>
+  </si>
+  <si>
+    <t>Min:57,12; Max:66,77; Med:60,45; DVPAD:2,80</t>
   </si>
   <si>
     <t>Min:2,01; Max:2,34; Med:2,18; DVPAD:0,12</t>
@@ -2212,7 +2204,7 @@
     <t>areolada</t>
   </si>
   <si>
-    <t>DIÂMETRO Min:33,31; Max:42,63; Med:37,47; DVPAD:2,87</t>
+    <t>Min:33,31; Max:42,63; Med:37,47; DVPAD:2,87</t>
   </si>
   <si>
     <t>Min:1,24; Max:1,61; Med:1,43; DVPAD:0,13</t>
@@ -2239,7 +2231,7 @@
     <t xml:space="preserve">Políade </t>
   </si>
   <si>
-    <t>DIÂMETRO Min:35,22; Max:50,06; Med:40,91; DVPAD:3,86</t>
+    <t>Min:35,22; Max:50,06; Med:40,91; DVPAD:3,86</t>
   </si>
   <si>
     <t>Min:1,33; Max:1,65; Med:1,51; DVPAD:0,10</t>
@@ -2473,7 +2465,7 @@
     <t>prolato-esferoidal a subprolato</t>
   </si>
   <si>
-    <t>Min1,03:; Max:1,22; Med:1,12; DVPAD:0,05</t>
+    <t>Min:1,03:; Max:1,22; Med:1,12; DVPAD:0,05</t>
   </si>
   <si>
     <t>Min:26,18; Max:36,18; Med:31,22; DVPAD:2,56</t>
@@ -2851,7 +2843,7 @@
     <t>psilada</t>
   </si>
   <si>
-    <t>DIÂMETRO Min:37,56; Max:48,72; Med:43,11; DVPAD:3,04</t>
+    <t>Min:37,56; Max:48,72; Med:43,11; DVPAD:3,04</t>
   </si>
   <si>
     <t>Min:1,16; Max:1,38; Med:1,26; DVPAD:0,05</t>
@@ -3231,7 +3223,7 @@
     <t>Min:0,69; Max:0,82; Med:0,76; DVPAD:0,03</t>
   </si>
   <si>
-    <t>Min:50,14 Max:59,98; Med:54,70; DVPAD:2,72</t>
+    <t>Min:50,14; Max:59,98; Med:54,70; DVPAD:2,72</t>
   </si>
   <si>
     <t>Min:62,89; Max:78,84; Med:72,24; DVPAD:3,95</t>
@@ -4087,7 +4079,7 @@
     <t>monoporado</t>
   </si>
   <si>
-    <t>DIÂMETRO Min:34,69; Max:42,74; Med:38,90; DVPAD:2,18</t>
+    <t>Min:34,69; Max:42,74; Med:38,90; DVPAD:2,18</t>
   </si>
   <si>
     <t>Min:1,39; Max:1,97; Med:1,70; DVPAD:0,17</t>
@@ -4949,7 +4941,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -5022,7 +5014,7 @@
     <xf numFmtId="49" fontId="6" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -5030,9 +5022,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -5073,9 +5062,6 @@
     <xf numFmtId="49" fontId="6" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -5085,31 +5071,28 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -5288,13 +5271,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -5384,7 +5361,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -5393,10 +5370,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -5651,13 +5628,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -5961,7 +5932,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -5970,10 +5941,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -6245,32 +6216,32 @@
     <col min="13" max="13" width="18" style="1" customWidth="1"/>
     <col min="14" max="14" width="13.6719" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.9531" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.8516" style="1" customWidth="1"/>
     <col min="18" max="18" width="31.1719" style="1" customWidth="1"/>
     <col min="19" max="19" width="20.6719" style="1" customWidth="1"/>
-    <col min="20" max="20" width="19.4453" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" style="1" customWidth="1"/>
     <col min="21" max="21" width="20.6719" style="1" customWidth="1"/>
     <col min="22" max="22" width="17.8516" style="1" customWidth="1"/>
     <col min="23" max="23" width="76.5" style="1" customWidth="1"/>
-    <col min="24" max="24" width="25.4688" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.9609" style="1" customWidth="1"/>
+    <col min="24" max="24" width="25.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16" style="1" customWidth="1"/>
     <col min="26" max="26" width="94.1719" style="1" customWidth="1"/>
-    <col min="27" max="27" width="17.3984" style="1" customWidth="1"/>
+    <col min="27" max="27" width="17.3516" style="1" customWidth="1"/>
     <col min="28" max="28" width="21.1719" style="1" customWidth="1"/>
-    <col min="29" max="29" width="18.7891" style="1" customWidth="1"/>
+    <col min="29" max="29" width="18.8516" style="1" customWidth="1"/>
     <col min="30" max="30" width="22.5" style="1" customWidth="1"/>
-    <col min="31" max="31" width="17.8203" style="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5547" style="1" customWidth="1"/>
-    <col min="33" max="33" width="17.5859" style="1" customWidth="1"/>
+    <col min="31" max="31" width="17.8516" style="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5" style="1" customWidth="1"/>
+    <col min="33" max="33" width="17.6719" style="1" customWidth="1"/>
     <col min="34" max="34" width="17" style="1" customWidth="1"/>
-    <col min="35" max="35" width="18.3281" style="1" customWidth="1"/>
-    <col min="36" max="36" width="18.0938" style="1" customWidth="1"/>
+    <col min="35" max="35" width="18.3516" style="1" customWidth="1"/>
+    <col min="36" max="36" width="18.1719" style="1" customWidth="1"/>
     <col min="37" max="37" width="21.8516" style="1" customWidth="1"/>
-    <col min="38" max="38" width="17.4219" style="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5" style="1" customWidth="1"/>
     <col min="39" max="39" width="18.6719" style="1" customWidth="1"/>
-    <col min="40" max="40" width="17.1562" style="1" customWidth="1"/>
-    <col min="41" max="41" width="18.2422" style="1" customWidth="1"/>
+    <col min="40" max="40" width="17.1719" style="1" customWidth="1"/>
+    <col min="41" max="41" width="18.3516" style="1" customWidth="1"/>
     <col min="42" max="42" width="20.3516" style="1" customWidth="1"/>
     <col min="43" max="43" width="96.8516" style="1" customWidth="1"/>
     <col min="44" max="44" width="41.3516" style="1" customWidth="1"/>
@@ -6285,11 +6256,11 @@
     <col min="53" max="53" width="52" style="1" customWidth="1"/>
     <col min="54" max="54" width="35.6719" style="1" customWidth="1"/>
     <col min="55" max="55" width="255" style="1" customWidth="1"/>
-    <col min="56" max="56" width="42.6328" style="1" customWidth="1"/>
+    <col min="56" max="56" width="42.6719" style="1" customWidth="1"/>
     <col min="57" max="57" width="27.8516" style="1" customWidth="1"/>
     <col min="58" max="58" width="25.5" style="1" customWidth="1"/>
     <col min="59" max="59" width="26.3516" style="1" customWidth="1"/>
-    <col min="60" max="60" width="20.5859" style="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6719" style="1" customWidth="1"/>
     <col min="61" max="61" width="21.3516" style="1" customWidth="1"/>
     <col min="62" max="256" width="18.1719" style="1" customWidth="1"/>
   </cols>
@@ -7710,7 +7681,7 @@
       <c r="AZ8" t="s" s="14">
         <v>224</v>
       </c>
-      <c r="BA8" s="27"/>
+      <c r="BA8" s="22"/>
       <c r="BB8" t="s" s="14">
         <v>225</v>
       </c>
@@ -7889,7 +7860,7 @@
         <v>241</v>
       </c>
       <c r="BD9" s="22"/>
-      <c r="BE9" s="28"/>
+      <c r="BE9" s="27"/>
       <c r="BF9" t="s" s="16">
         <v>242</v>
       </c>
@@ -8071,7 +8042,7 @@
       </c>
     </row>
     <row r="11" ht="17" customHeight="1">
-      <c r="A11" s="29"/>
+      <c r="A11" s="28"/>
       <c r="B11" t="s" s="14">
         <v>136</v>
       </c>
@@ -8144,7 +8115,7 @@
       <c r="Y11" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z11" s="30"/>
+      <c r="Z11" s="29"/>
       <c r="AA11" t="s" s="21">
         <v>249</v>
       </c>
@@ -8223,7 +8194,7 @@
       <c r="BB11" t="s" s="14">
         <v>270</v>
       </c>
-      <c r="BC11" s="31"/>
+      <c r="BC11" s="30"/>
       <c r="BD11" s="22"/>
       <c r="BE11" t="s" s="16">
         <v>271</v>
@@ -8238,7 +8209,7 @@
       </c>
     </row>
     <row r="12" ht="17" customHeight="1">
-      <c r="A12" s="29"/>
+      <c r="A12" s="28"/>
       <c r="B12" t="s" s="14">
         <v>136</v>
       </c>
@@ -8311,7 +8282,7 @@
       <c r="Y12" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z12" s="30"/>
+      <c r="Z12" s="29"/>
       <c r="AA12" t="s" s="21">
         <v>249</v>
       </c>
@@ -8407,7 +8378,7 @@
       </c>
     </row>
     <row r="13" ht="17" customHeight="1">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
       <c r="B13" t="s" s="14">
         <v>136</v>
       </c>
@@ -8480,7 +8451,7 @@
       <c r="Y13" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z13" s="30"/>
+      <c r="Z13" s="29"/>
       <c r="AA13" t="s" s="21">
         <v>292</v>
       </c>
@@ -8559,7 +8530,7 @@
       <c r="BB13" t="s" s="14">
         <v>300</v>
       </c>
-      <c r="BC13" s="31"/>
+      <c r="BC13" s="30"/>
       <c r="BD13" s="22"/>
       <c r="BE13" t="s" s="16">
         <v>301</v>
@@ -8574,7 +8545,7 @@
       </c>
     </row>
     <row r="14" ht="17" customHeight="1">
-      <c r="A14" s="29"/>
+      <c r="A14" s="28"/>
       <c r="B14" t="s" s="14">
         <v>136</v>
       </c>
@@ -8647,7 +8618,7 @@
       <c r="Y14" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z14" s="30"/>
+      <c r="Z14" s="29"/>
       <c r="AA14" t="s" s="21">
         <v>158</v>
       </c>
@@ -8745,7 +8716,7 @@
       </c>
     </row>
     <row r="15" ht="17" customHeight="1">
-      <c r="A15" s="29"/>
+      <c r="A15" s="28"/>
       <c r="B15" t="s" s="14">
         <v>136</v>
       </c>
@@ -8818,7 +8789,7 @@
       <c r="Y15" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z15" s="30"/>
+      <c r="Z15" s="29"/>
       <c r="AA15" t="s" s="21">
         <v>158</v>
       </c>
@@ -8897,7 +8868,7 @@
       <c r="BB15" t="s" s="14">
         <v>325</v>
       </c>
-      <c r="BC15" s="31"/>
+      <c r="BC15" s="30"/>
       <c r="BD15" s="22"/>
       <c r="BE15" t="s" s="16">
         <v>326</v>
@@ -8912,7 +8883,7 @@
       </c>
     </row>
     <row r="16" ht="17" customHeight="1">
-      <c r="A16" s="29"/>
+      <c r="A16" s="28"/>
       <c r="B16" t="s" s="14">
         <v>136</v>
       </c>
@@ -8931,10 +8902,10 @@
       <c r="G16" t="s" s="16">
         <v>304</v>
       </c>
-      <c r="H16" t="s" s="32">
+      <c r="H16" t="s" s="31">
         <v>329</v>
       </c>
-      <c r="I16" t="s" s="33">
+      <c r="I16" t="s" s="32">
         <v>330</v>
       </c>
       <c r="J16" t="s" s="18">
@@ -8985,7 +8956,7 @@
       <c r="Y16" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z16" s="34"/>
+      <c r="Z16" s="33"/>
       <c r="AA16" t="s" s="21">
         <v>249</v>
       </c>
@@ -9083,7 +9054,7 @@
       </c>
     </row>
     <row r="17" ht="17" customHeight="1">
-      <c r="A17" s="29"/>
+      <c r="A17" s="28"/>
       <c r="B17" t="s" s="14">
         <v>136</v>
       </c>
@@ -9156,7 +9127,7 @@
       <c r="Y17" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z17" s="30"/>
+      <c r="Z17" s="29"/>
       <c r="AA17" t="s" s="21">
         <v>158</v>
       </c>
@@ -9254,7 +9225,7 @@
       </c>
     </row>
     <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="29"/>
+      <c r="A18" s="28"/>
       <c r="B18" t="s" s="14">
         <v>136</v>
       </c>
@@ -9327,7 +9298,7 @@
       <c r="Y18" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z18" s="30"/>
+      <c r="Z18" s="29"/>
       <c r="AA18" t="s" s="21">
         <v>292</v>
       </c>
@@ -9423,7 +9394,7 @@
       </c>
     </row>
     <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="29"/>
+      <c r="A19" s="28"/>
       <c r="B19" t="s" s="14">
         <v>136</v>
       </c>
@@ -9442,10 +9413,10 @@
       <c r="G19" t="s" s="16">
         <v>365</v>
       </c>
-      <c r="H19" t="s" s="35">
+      <c r="H19" t="s" s="34">
         <v>366</v>
       </c>
-      <c r="I19" t="s" s="36">
+      <c r="I19" t="s" s="35">
         <v>367</v>
       </c>
       <c r="J19" t="s" s="18">
@@ -9496,7 +9467,7 @@
       <c r="Y19" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z19" s="30"/>
+      <c r="Z19" s="29"/>
       <c r="AA19" t="s" s="21">
         <v>249</v>
       </c>
@@ -9592,7 +9563,7 @@
       </c>
     </row>
     <row r="20" ht="17" customHeight="1">
-      <c r="A20" s="29"/>
+      <c r="A20" s="28"/>
       <c r="B20" t="s" s="14">
         <v>136</v>
       </c>
@@ -9665,7 +9636,7 @@
       <c r="Y20" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z20" s="30"/>
+      <c r="Z20" s="29"/>
       <c r="AA20" t="s" s="21">
         <v>249</v>
       </c>
@@ -9761,7 +9732,7 @@
       </c>
     </row>
     <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="29"/>
+      <c r="A21" s="28"/>
       <c r="B21" t="s" s="14">
         <v>136</v>
       </c>
@@ -9834,7 +9805,7 @@
       <c r="Y21" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z21" s="34"/>
+      <c r="Z21" s="33"/>
       <c r="AA21" t="s" s="21">
         <v>249</v>
       </c>
@@ -9930,7 +9901,7 @@
       </c>
     </row>
     <row r="22" ht="17" customHeight="1">
-      <c r="A22" s="29"/>
+      <c r="A22" s="28"/>
       <c r="B22" t="s" s="14">
         <v>136</v>
       </c>
@@ -9949,10 +9920,10 @@
       <c r="G22" t="s" s="16">
         <v>365</v>
       </c>
-      <c r="H22" t="s" s="32">
+      <c r="H22" t="s" s="31">
         <v>405</v>
       </c>
-      <c r="I22" t="s" s="33">
+      <c r="I22" t="s" s="32">
         <v>406</v>
       </c>
       <c r="J22" t="s" s="18">
@@ -10003,7 +9974,7 @@
       <c r="Y22" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z22" s="34"/>
+      <c r="Z22" s="33"/>
       <c r="AA22" t="s" s="21">
         <v>249</v>
       </c>
@@ -10082,7 +10053,7 @@
       <c r="BB22" t="s" s="14">
         <v>411</v>
       </c>
-      <c r="BC22" s="31"/>
+      <c r="BC22" s="30"/>
       <c r="BD22" s="26"/>
       <c r="BE22" t="s" s="16">
         <v>412</v>
@@ -10097,7 +10068,7 @@
       </c>
     </row>
     <row r="23" ht="17" customHeight="1">
-      <c r="A23" s="29"/>
+      <c r="A23" s="28"/>
       <c r="B23" t="s" s="14">
         <v>136</v>
       </c>
@@ -10170,7 +10141,7 @@
       <c r="Y23" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z23" s="30"/>
+      <c r="Z23" s="29"/>
       <c r="AA23" t="s" s="21">
         <v>249</v>
       </c>
@@ -10249,7 +10220,7 @@
       <c r="BB23" t="s" s="14">
         <v>425</v>
       </c>
-      <c r="BC23" s="31"/>
+      <c r="BC23" s="30"/>
       <c r="BD23" s="26"/>
       <c r="BE23" t="s" s="16">
         <v>426</v>
@@ -10264,7 +10235,7 @@
       </c>
     </row>
     <row r="24" ht="17" customHeight="1">
-      <c r="A24" s="29"/>
+      <c r="A24" s="28"/>
       <c r="B24" t="s" s="14">
         <v>136</v>
       </c>
@@ -10337,7 +10308,7 @@
       <c r="Y24" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z24" s="30"/>
+      <c r="Z24" s="29"/>
       <c r="AA24" t="s" s="21">
         <v>249</v>
       </c>
@@ -10416,7 +10387,7 @@
       <c r="BB24" t="s" s="14">
         <v>441</v>
       </c>
-      <c r="BC24" s="31"/>
+      <c r="BC24" s="30"/>
       <c r="BD24" s="26"/>
       <c r="BE24" t="s" s="16">
         <v>442</v>
@@ -10431,7 +10402,7 @@
       </c>
     </row>
     <row r="25" ht="17" customHeight="1">
-      <c r="A25" s="29"/>
+      <c r="A25" s="28"/>
       <c r="B25" t="s" s="14">
         <v>136</v>
       </c>
@@ -10450,10 +10421,10 @@
       <c r="G25" t="s" s="16">
         <v>445</v>
       </c>
-      <c r="H25" t="s" s="37">
+      <c r="H25" t="s" s="36">
         <v>446</v>
       </c>
-      <c r="I25" t="s" s="38">
+      <c r="I25" t="s" s="37">
         <v>447</v>
       </c>
       <c r="J25" t="s" s="18">
@@ -10504,7 +10475,7 @@
       <c r="Y25" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z25" s="30"/>
+      <c r="Z25" s="29"/>
       <c r="AA25" t="s" s="21">
         <v>249</v>
       </c>
@@ -10600,7 +10571,7 @@
       </c>
     </row>
     <row r="26" ht="17" customHeight="1">
-      <c r="A26" s="29"/>
+      <c r="A26" s="28"/>
       <c r="B26" t="s" s="14">
         <v>136</v>
       </c>
@@ -10673,7 +10644,7 @@
       <c r="Y26" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z26" s="30"/>
+      <c r="Z26" s="29"/>
       <c r="AA26" t="s" s="21">
         <v>249</v>
       </c>
@@ -10769,7 +10740,7 @@
       </c>
     </row>
     <row r="27" ht="17" customHeight="1">
-      <c r="A27" s="29"/>
+      <c r="A27" s="28"/>
       <c r="B27" t="s" s="14">
         <v>136</v>
       </c>
@@ -10842,7 +10813,7 @@
       <c r="Y27" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z27" s="30"/>
+      <c r="Z27" s="29"/>
       <c r="AA27" t="s" s="21">
         <v>249</v>
       </c>
@@ -10921,7 +10892,7 @@
       <c r="BB27" t="s" s="14">
         <v>484</v>
       </c>
-      <c r="BC27" s="31"/>
+      <c r="BC27" s="30"/>
       <c r="BD27" s="26"/>
       <c r="BE27" t="s" s="16">
         <v>485</v>
@@ -10936,7 +10907,7 @@
       </c>
     </row>
     <row r="28" ht="17" customHeight="1">
-      <c r="A28" s="29"/>
+      <c r="A28" s="28"/>
       <c r="B28" t="s" s="14">
         <v>136</v>
       </c>
@@ -11009,7 +10980,7 @@
       <c r="Y28" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z28" s="30"/>
+      <c r="Z28" s="29"/>
       <c r="AA28" t="s" s="21">
         <v>249</v>
       </c>
@@ -11070,7 +11041,7 @@
       <c r="AT28" t="s" s="21">
         <v>177</v>
       </c>
-      <c r="AU28" t="s" s="39">
+      <c r="AU28" t="s" s="38">
         <v>252</v>
       </c>
       <c r="AV28" t="s" s="14">
@@ -11088,7 +11059,7 @@
       <c r="BB28" t="s" s="14">
         <v>498</v>
       </c>
-      <c r="BC28" s="31"/>
+      <c r="BC28" s="30"/>
       <c r="BD28" s="26"/>
       <c r="BE28" t="s" s="16">
         <v>499</v>
@@ -11103,7 +11074,7 @@
       </c>
     </row>
     <row r="29" ht="17" customHeight="1">
-      <c r="A29" s="29"/>
+      <c r="A29" s="28"/>
       <c r="B29" t="s" s="14">
         <v>136</v>
       </c>
@@ -11176,7 +11147,7 @@
       <c r="Y29" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z29" s="30"/>
+      <c r="Z29" s="29"/>
       <c r="AA29" t="s" s="21">
         <v>249</v>
       </c>
@@ -11255,7 +11226,7 @@
       <c r="BB29" t="s" s="14">
         <v>513</v>
       </c>
-      <c r="BC29" s="31"/>
+      <c r="BC29" s="30"/>
       <c r="BD29" s="26"/>
       <c r="BE29" t="s" s="16">
         <v>514</v>
@@ -11270,7 +11241,7 @@
       </c>
     </row>
     <row r="30" ht="17" customHeight="1">
-      <c r="A30" s="29"/>
+      <c r="A30" s="28"/>
       <c r="B30" t="s" s="14">
         <v>136</v>
       </c>
@@ -11343,7 +11314,7 @@
       <c r="Y30" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z30" s="30"/>
+      <c r="Z30" s="29"/>
       <c r="AA30" t="s" s="21">
         <v>249</v>
       </c>
@@ -11422,7 +11393,7 @@
       <c r="BB30" t="s" s="14">
         <v>524</v>
       </c>
-      <c r="BC30" s="31"/>
+      <c r="BC30" s="30"/>
       <c r="BD30" s="26"/>
       <c r="BE30" t="s" s="16">
         <v>525</v>
@@ -11437,7 +11408,7 @@
       </c>
     </row>
     <row r="31" ht="17" customHeight="1">
-      <c r="A31" s="29"/>
+      <c r="A31" s="28"/>
       <c r="B31" t="s" s="14">
         <v>136</v>
       </c>
@@ -11510,7 +11481,7 @@
       <c r="Y31" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z31" s="30"/>
+      <c r="Z31" s="29"/>
       <c r="AA31" t="s" s="21">
         <v>292</v>
       </c>
@@ -11589,7 +11560,7 @@
       <c r="BB31" t="s" s="14">
         <v>535</v>
       </c>
-      <c r="BC31" t="s" s="40">
+      <c r="BC31" t="s" s="39">
         <v>536</v>
       </c>
       <c r="BD31" s="26"/>
@@ -11606,7 +11577,7 @@
       </c>
     </row>
     <row r="32" ht="17" customHeight="1">
-      <c r="A32" s="29"/>
+      <c r="A32" s="28"/>
       <c r="B32" t="s" s="14">
         <v>136</v>
       </c>
@@ -11679,7 +11650,7 @@
       <c r="Y32" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z32" s="30"/>
+      <c r="Z32" s="29"/>
       <c r="AA32" t="s" s="21">
         <v>158</v>
       </c>
@@ -11750,11 +11721,11 @@
       <c r="AZ32" t="s" s="14">
         <v>546</v>
       </c>
-      <c r="BA32" s="41"/>
+      <c r="BA32" s="40"/>
       <c r="BB32" t="s" s="14">
         <v>547</v>
       </c>
-      <c r="BC32" s="31"/>
+      <c r="BC32" s="30"/>
       <c r="BD32" s="26"/>
       <c r="BE32" t="s" s="16">
         <v>548</v>
@@ -11769,7 +11740,7 @@
       </c>
     </row>
     <row r="33" ht="17" customHeight="1">
-      <c r="A33" s="29"/>
+      <c r="A33" s="28"/>
       <c r="B33" t="s" s="14">
         <v>136</v>
       </c>
@@ -11788,10 +11759,10 @@
       <c r="G33" t="s" s="16">
         <v>551</v>
       </c>
-      <c r="H33" t="s" s="38">
+      <c r="H33" t="s" s="37">
         <v>552</v>
       </c>
-      <c r="I33" t="s" s="38">
+      <c r="I33" t="s" s="37">
         <v>553</v>
       </c>
       <c r="J33" t="s" s="18">
@@ -11842,7 +11813,7 @@
       <c r="Y33" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z33" s="30"/>
+      <c r="Z33" s="29"/>
       <c r="AA33" t="s" s="21">
         <v>158</v>
       </c>
@@ -11891,7 +11862,7 @@
       <c r="AP33" t="s" s="21">
         <v>559</v>
       </c>
-      <c r="AQ33" s="42"/>
+      <c r="AQ33" s="40"/>
       <c r="AR33" t="s" s="21">
         <v>560</v>
       </c>
@@ -11917,7 +11888,7 @@
       <c r="BB33" t="s" s="14">
         <v>563</v>
       </c>
-      <c r="BC33" s="31"/>
+      <c r="BC33" s="30"/>
       <c r="BD33" s="26"/>
       <c r="BE33" t="s" s="16">
         <v>564</v>
@@ -11925,14 +11896,14 @@
       <c r="BF33" t="s" s="16">
         <v>565</v>
       </c>
-      <c r="BG33" s="43"/>
+      <c r="BG33" s="41"/>
       <c r="BH33" s="26"/>
       <c r="BI33" t="s" s="16">
         <v>566</v>
       </c>
     </row>
     <row r="34" ht="17" customHeight="1">
-      <c r="A34" s="29"/>
+      <c r="A34" s="28"/>
       <c r="B34" t="s" s="14">
         <v>136</v>
       </c>
@@ -12005,7 +11976,7 @@
       <c r="Y34" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z34" s="30"/>
+      <c r="Z34" s="29"/>
       <c r="AA34" t="s" s="21">
         <v>292</v>
       </c>
@@ -12084,7 +12055,7 @@
       <c r="BB34" t="s" s="14">
         <v>576</v>
       </c>
-      <c r="BC34" t="s" s="40">
+      <c r="BC34" t="s" s="39">
         <v>577</v>
       </c>
       <c r="BD34" s="26"/>
@@ -12101,7 +12072,7 @@
       </c>
     </row>
     <row r="35" ht="17" customHeight="1">
-      <c r="A35" s="29"/>
+      <c r="A35" s="28"/>
       <c r="B35" t="s" s="14">
         <v>136</v>
       </c>
@@ -12174,7 +12145,7 @@
       <c r="Y35" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z35" s="30"/>
+      <c r="Z35" s="29"/>
       <c r="AA35" t="s" s="21">
         <v>158</v>
       </c>
@@ -12253,7 +12224,7 @@
       <c r="BB35" t="s" s="14">
         <v>588</v>
       </c>
-      <c r="BC35" s="31"/>
+      <c r="BC35" s="30"/>
       <c r="BD35" s="26"/>
       <c r="BE35" t="s" s="16">
         <v>589</v>
@@ -12268,7 +12239,7 @@
       </c>
     </row>
     <row r="36" ht="17" customHeight="1">
-      <c r="A36" s="29"/>
+      <c r="A36" s="28"/>
       <c r="B36" t="s" s="14">
         <v>136</v>
       </c>
@@ -12341,7 +12312,7 @@
       <c r="Y36" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z36" s="30"/>
+      <c r="Z36" s="29"/>
       <c r="AA36" t="s" s="21">
         <v>249</v>
       </c>
@@ -12420,7 +12391,7 @@
       <c r="BB36" t="s" s="14">
         <v>599</v>
       </c>
-      <c r="BC36" s="31"/>
+      <c r="BC36" s="30"/>
       <c r="BD36" s="26"/>
       <c r="BE36" t="s" s="16">
         <v>600</v>
@@ -12435,7 +12406,7 @@
       </c>
     </row>
     <row r="37" ht="17" customHeight="1">
-      <c r="A37" s="29"/>
+      <c r="A37" s="28"/>
       <c r="B37" t="s" s="14">
         <v>136</v>
       </c>
@@ -12508,7 +12479,7 @@
       <c r="Y37" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z37" s="34"/>
+      <c r="Z37" s="33"/>
       <c r="AA37" t="s" s="21">
         <v>249</v>
       </c>
@@ -12548,8 +12519,8 @@
       <c r="AM37" t="s" s="21">
         <v>608</v>
       </c>
-      <c r="AN37" s="42"/>
-      <c r="AO37" s="42"/>
+      <c r="AN37" s="40"/>
+      <c r="AO37" s="40"/>
       <c r="AP37" t="s" s="21">
         <v>609</v>
       </c>
@@ -12575,11 +12546,11 @@
       <c r="AZ37" t="s" s="14">
         <v>613</v>
       </c>
-      <c r="BA37" s="41"/>
+      <c r="BA37" s="40"/>
       <c r="BB37" t="s" s="14">
         <v>614</v>
       </c>
-      <c r="BC37" s="31"/>
+      <c r="BC37" s="30"/>
       <c r="BD37" s="26"/>
       <c r="BE37" t="s" s="16">
         <v>615</v>
@@ -12594,7 +12565,7 @@
       </c>
     </row>
     <row r="38" ht="17" customHeight="1">
-      <c r="A38" s="29"/>
+      <c r="A38" s="28"/>
       <c r="B38" t="s" s="14">
         <v>136</v>
       </c>
@@ -12667,7 +12638,7 @@
       <c r="Y38" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z38" s="34"/>
+      <c r="Z38" s="33"/>
       <c r="AA38" t="s" s="21">
         <v>249</v>
       </c>
@@ -12707,8 +12678,8 @@
       <c r="AM38" t="s" s="21">
         <v>621</v>
       </c>
-      <c r="AN38" s="42"/>
-      <c r="AO38" s="42"/>
+      <c r="AN38" s="40"/>
+      <c r="AO38" s="40"/>
       <c r="AP38" t="s" s="21">
         <v>609</v>
       </c>
@@ -12738,7 +12709,7 @@
       <c r="BB38" t="s" s="14">
         <v>623</v>
       </c>
-      <c r="BC38" s="31"/>
+      <c r="BC38" s="30"/>
       <c r="BD38" s="26"/>
       <c r="BE38" t="s" s="16">
         <v>624</v>
@@ -12753,7 +12724,7 @@
       </c>
     </row>
     <row r="39" ht="17" customHeight="1">
-      <c r="A39" s="29"/>
+      <c r="A39" s="28"/>
       <c r="B39" t="s" s="14">
         <v>136</v>
       </c>
@@ -12826,7 +12797,7 @@
       <c r="Y39" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z39" s="30"/>
+      <c r="Z39" s="29"/>
       <c r="AA39" t="s" s="21">
         <v>249</v>
       </c>
@@ -12905,7 +12876,7 @@
       <c r="BB39" t="s" s="14">
         <v>639</v>
       </c>
-      <c r="BC39" s="31"/>
+      <c r="BC39" s="30"/>
       <c r="BD39" s="26"/>
       <c r="BE39" t="s" s="16">
         <v>640</v>
@@ -12920,7 +12891,7 @@
       </c>
     </row>
     <row r="40" ht="17" customHeight="1">
-      <c r="A40" s="29"/>
+      <c r="A40" s="28"/>
       <c r="B40" t="s" s="14">
         <v>136</v>
       </c>
@@ -12993,7 +12964,7 @@
       <c r="Y40" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z40" s="34"/>
+      <c r="Z40" s="33"/>
       <c r="AA40" t="s" s="21">
         <v>249</v>
       </c>
@@ -13072,7 +13043,7 @@
       <c r="BB40" t="s" s="14">
         <v>651</v>
       </c>
-      <c r="BC40" t="s" s="40">
+      <c r="BC40" t="s" s="39">
         <v>652</v>
       </c>
       <c r="BD40" s="26"/>
@@ -13091,7 +13062,7 @@
       </c>
     </row>
     <row r="41" ht="17" customHeight="1">
-      <c r="A41" s="29"/>
+      <c r="A41" s="28"/>
       <c r="B41" t="s" s="14">
         <v>136</v>
       </c>
@@ -13164,7 +13135,7 @@
       <c r="Y41" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z41" s="34"/>
+      <c r="Z41" s="33"/>
       <c r="AA41" t="s" s="21">
         <v>292</v>
       </c>
@@ -13243,7 +13214,7 @@
       <c r="BB41" t="s" s="14">
         <v>665</v>
       </c>
-      <c r="BC41" t="s" s="40">
+      <c r="BC41" t="s" s="39">
         <v>666</v>
       </c>
       <c r="BD41" s="26"/>
@@ -13262,7 +13233,7 @@
       </c>
     </row>
     <row r="42" ht="17" customHeight="1">
-      <c r="A42" s="29"/>
+      <c r="A42" s="28"/>
       <c r="B42" t="s" s="14">
         <v>136</v>
       </c>
@@ -13335,7 +13306,7 @@
       <c r="Y42" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z42" s="30"/>
+      <c r="Z42" s="29"/>
       <c r="AA42" t="s" s="21">
         <v>249</v>
       </c>
@@ -13414,7 +13385,7 @@
       <c r="BB42" t="s" s="14">
         <v>679</v>
       </c>
-      <c r="BC42" t="s" s="40">
+      <c r="BC42" t="s" s="39">
         <v>680</v>
       </c>
       <c r="BD42" s="26"/>
@@ -13433,7 +13404,7 @@
       </c>
     </row>
     <row r="43" ht="17" customHeight="1">
-      <c r="A43" s="29"/>
+      <c r="A43" s="28"/>
       <c r="B43" t="s" s="14">
         <v>136</v>
       </c>
@@ -13506,7 +13477,7 @@
       <c r="Y43" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z43" s="30"/>
+      <c r="Z43" s="29"/>
       <c r="AA43" t="s" s="21">
         <v>249</v>
       </c>
@@ -13585,7 +13556,7 @@
       <c r="BB43" t="s" s="14">
         <v>691</v>
       </c>
-      <c r="BC43" s="31"/>
+      <c r="BC43" s="30"/>
       <c r="BD43" s="26"/>
       <c r="BE43" t="s" s="16">
         <v>692</v>
@@ -13600,7 +13571,7 @@
       </c>
     </row>
     <row r="44" ht="17" customHeight="1">
-      <c r="A44" s="29"/>
+      <c r="A44" s="28"/>
       <c r="B44" t="s" s="14">
         <v>136</v>
       </c>
@@ -13673,7 +13644,7 @@
       <c r="Y44" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z44" s="30"/>
+      <c r="Z44" s="29"/>
       <c r="AA44" t="s" s="21">
         <v>249</v>
       </c>
@@ -13752,7 +13723,7 @@
       <c r="BB44" t="s" s="14">
         <v>703</v>
       </c>
-      <c r="BC44" s="31"/>
+      <c r="BC44" s="30"/>
       <c r="BD44" s="26"/>
       <c r="BE44" t="s" s="16">
         <v>704</v>
@@ -13767,7 +13738,7 @@
       </c>
     </row>
     <row r="45" ht="17" customHeight="1">
-      <c r="A45" s="29"/>
+      <c r="A45" s="28"/>
       <c r="B45" t="s" s="14">
         <v>136</v>
       </c>
@@ -13840,7 +13811,7 @@
       <c r="Y45" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z45" s="30"/>
+      <c r="Z45" s="29"/>
       <c r="AA45" t="s" s="21">
         <v>158</v>
       </c>
@@ -13919,7 +13890,7 @@
       <c r="BB45" t="s" s="14">
         <v>716</v>
       </c>
-      <c r="BC45" t="s" s="40">
+      <c r="BC45" t="s" s="39">
         <v>717</v>
       </c>
       <c r="BD45" s="26"/>
@@ -13936,7 +13907,7 @@
       </c>
     </row>
     <row r="46" ht="17" customHeight="1">
-      <c r="A46" s="29"/>
+      <c r="A46" s="28"/>
       <c r="B46" t="s" s="14">
         <v>136</v>
       </c>
@@ -14009,7 +13980,7 @@
       <c r="Y46" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z46" s="30"/>
+      <c r="Z46" s="29"/>
       <c r="AA46" t="s" s="21">
         <v>158</v>
       </c>
@@ -14088,7 +14059,7 @@
       <c r="BB46" t="s" s="14">
         <v>730</v>
       </c>
-      <c r="BC46" t="s" s="40">
+      <c r="BC46" t="s" s="39">
         <v>731</v>
       </c>
       <c r="BD46" s="26"/>
@@ -14105,7 +14076,7 @@
       </c>
     </row>
     <row r="47" ht="17" customHeight="1">
-      <c r="A47" s="29"/>
+      <c r="A47" s="28"/>
       <c r="B47" t="s" s="14">
         <v>136</v>
       </c>
@@ -14178,7 +14149,7 @@
       <c r="Y47" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z47" s="34"/>
+      <c r="Z47" s="33"/>
       <c r="AA47" t="s" s="21">
         <v>249</v>
       </c>
@@ -14257,7 +14228,7 @@
       <c r="BB47" t="s" s="14">
         <v>743</v>
       </c>
-      <c r="BC47" t="s" s="40">
+      <c r="BC47" t="s" s="39">
         <v>208</v>
       </c>
       <c r="BD47" s="26"/>
@@ -14274,7 +14245,7 @@
       </c>
     </row>
     <row r="48" ht="17" customHeight="1">
-      <c r="A48" s="29"/>
+      <c r="A48" s="28"/>
       <c r="B48" t="s" s="14">
         <v>136</v>
       </c>
@@ -14347,7 +14318,7 @@
       <c r="Y48" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z48" s="30"/>
+      <c r="Z48" s="29"/>
       <c r="AA48" t="s" s="21">
         <v>158</v>
       </c>
@@ -14426,7 +14397,7 @@
       <c r="BB48" t="s" s="14">
         <v>754</v>
       </c>
-      <c r="BC48" s="31"/>
+      <c r="BC48" s="30"/>
       <c r="BD48" s="26"/>
       <c r="BE48" t="s" s="16">
         <v>755</v>
@@ -14441,7 +14412,7 @@
       </c>
     </row>
     <row r="49" ht="17" customHeight="1">
-      <c r="A49" s="29"/>
+      <c r="A49" s="28"/>
       <c r="B49" t="s" s="14">
         <v>136</v>
       </c>
@@ -14514,7 +14485,7 @@
       <c r="Y49" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z49" s="30"/>
+      <c r="Z49" s="29"/>
       <c r="AA49" t="s" s="21">
         <v>249</v>
       </c>
@@ -14593,7 +14564,7 @@
       <c r="BB49" t="s" s="14">
         <v>765</v>
       </c>
-      <c r="BC49" t="s" s="40">
+      <c r="BC49" t="s" s="39">
         <v>766</v>
       </c>
       <c r="BD49" s="26"/>
@@ -14610,7 +14581,7 @@
       </c>
     </row>
     <row r="50" ht="17" customHeight="1">
-      <c r="A50" s="29"/>
+      <c r="A50" s="28"/>
       <c r="B50" t="s" s="14">
         <v>136</v>
       </c>
@@ -14629,10 +14600,10 @@
       <c r="G50" t="s" s="16">
         <v>603</v>
       </c>
-      <c r="H50" t="s" s="44">
+      <c r="H50" t="s" s="42">
         <v>770</v>
       </c>
-      <c r="I50" t="s" s="38">
+      <c r="I50" t="s" s="37">
         <v>771</v>
       </c>
       <c r="J50" t="s" s="18">
@@ -14683,7 +14654,7 @@
       <c r="Y50" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z50" s="30"/>
+      <c r="Z50" s="29"/>
       <c r="AA50" t="s" s="21">
         <v>249</v>
       </c>
@@ -14762,7 +14733,7 @@
       <c r="BB50" t="s" s="14">
         <v>779</v>
       </c>
-      <c r="BC50" t="s" s="40">
+      <c r="BC50" t="s" s="39">
         <v>780</v>
       </c>
       <c r="BD50" s="26"/>
@@ -14781,7 +14752,7 @@
       </c>
     </row>
     <row r="51" ht="17" customHeight="1">
-      <c r="A51" s="29"/>
+      <c r="A51" s="28"/>
       <c r="B51" t="s" s="14">
         <v>136</v>
       </c>
@@ -14854,7 +14825,7 @@
       <c r="Y51" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z51" s="30"/>
+      <c r="Z51" s="29"/>
       <c r="AA51" t="s" s="21">
         <v>249</v>
       </c>
@@ -14933,7 +14904,7 @@
       <c r="BB51" t="s" s="14">
         <v>794</v>
       </c>
-      <c r="BC51" s="31"/>
+      <c r="BC51" s="30"/>
       <c r="BD51" s="26"/>
       <c r="BE51" t="s" s="16">
         <v>795</v>
@@ -14948,7 +14919,7 @@
       </c>
     </row>
     <row r="52" ht="17" customHeight="1">
-      <c r="A52" s="29"/>
+      <c r="A52" s="28"/>
       <c r="B52" t="s" s="14">
         <v>136</v>
       </c>
@@ -15021,7 +14992,7 @@
       <c r="Y52" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z52" s="30"/>
+      <c r="Z52" s="29"/>
       <c r="AA52" t="s" s="21">
         <v>249</v>
       </c>
@@ -15100,7 +15071,7 @@
       <c r="BB52" t="s" s="14">
         <v>805</v>
       </c>
-      <c r="BC52" t="s" s="40">
+      <c r="BC52" t="s" s="39">
         <v>806</v>
       </c>
       <c r="BD52" s="26"/>
@@ -15117,7 +15088,7 @@
       </c>
     </row>
     <row r="53" ht="17" customHeight="1">
-      <c r="A53" s="29"/>
+      <c r="A53" s="28"/>
       <c r="B53" t="s" s="14">
         <v>136</v>
       </c>
@@ -15190,7 +15161,7 @@
       <c r="Y53" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z53" s="30"/>
+      <c r="Z53" s="29"/>
       <c r="AA53" t="s" s="21">
         <v>249</v>
       </c>
@@ -15269,7 +15240,7 @@
       <c r="BB53" t="s" s="14">
         <v>817</v>
       </c>
-      <c r="BC53" s="31"/>
+      <c r="BC53" s="30"/>
       <c r="BD53" s="26"/>
       <c r="BE53" t="s" s="16">
         <v>818</v>
@@ -15284,7 +15255,7 @@
       </c>
     </row>
     <row r="54" ht="17" customHeight="1">
-      <c r="A54" s="29"/>
+      <c r="A54" s="28"/>
       <c r="B54" t="s" s="14">
         <v>136</v>
       </c>
@@ -15303,10 +15274,10 @@
       <c r="G54" t="s" s="16">
         <v>603</v>
       </c>
-      <c r="H54" t="s" s="32">
+      <c r="H54" t="s" s="31">
         <v>821</v>
       </c>
-      <c r="I54" t="s" s="33">
+      <c r="I54" t="s" s="32">
         <v>822</v>
       </c>
       <c r="J54" t="s" s="18">
@@ -15357,7 +15328,7 @@
       <c r="Y54" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z54" s="34"/>
+      <c r="Z54" s="33"/>
       <c r="AA54" t="s" s="21">
         <v>249</v>
       </c>
@@ -15397,8 +15368,8 @@
       <c r="AM54" t="s" s="21">
         <v>608</v>
       </c>
-      <c r="AN54" s="42"/>
-      <c r="AO54" s="42"/>
+      <c r="AN54" s="40"/>
+      <c r="AO54" s="40"/>
       <c r="AP54" t="s" s="21">
         <v>609</v>
       </c>
@@ -15424,11 +15395,11 @@
       <c r="AZ54" t="s" s="14">
         <v>826</v>
       </c>
-      <c r="BA54" s="41"/>
+      <c r="BA54" s="40"/>
       <c r="BB54" t="s" s="14">
         <v>827</v>
       </c>
-      <c r="BC54" s="31"/>
+      <c r="BC54" s="30"/>
       <c r="BD54" s="26"/>
       <c r="BE54" t="s" s="16">
         <v>828</v>
@@ -15443,7 +15414,7 @@
       </c>
     </row>
     <row r="55" ht="17" customHeight="1">
-      <c r="A55" s="29"/>
+      <c r="A55" s="28"/>
       <c r="B55" t="s" s="14">
         <v>136</v>
       </c>
@@ -15516,7 +15487,7 @@
       <c r="Y55" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z55" s="34"/>
+      <c r="Z55" s="33"/>
       <c r="AA55" t="s" s="21">
         <v>249</v>
       </c>
@@ -15595,7 +15566,7 @@
       <c r="BB55" t="s" s="14">
         <v>838</v>
       </c>
-      <c r="BC55" t="s" s="40">
+      <c r="BC55" t="s" s="39">
         <v>839</v>
       </c>
       <c r="BD55" s="26"/>
@@ -15612,7 +15583,7 @@
       </c>
     </row>
     <row r="56" ht="17" customHeight="1">
-      <c r="A56" s="29"/>
+      <c r="A56" s="28"/>
       <c r="B56" t="s" s="14">
         <v>136</v>
       </c>
@@ -15685,7 +15656,7 @@
       <c r="Y56" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z56" s="30"/>
+      <c r="Z56" s="29"/>
       <c r="AA56" t="s" s="21">
         <v>249</v>
       </c>
@@ -15764,7 +15735,7 @@
       <c r="BB56" t="s" s="14">
         <v>850</v>
       </c>
-      <c r="BC56" s="31"/>
+      <c r="BC56" s="30"/>
       <c r="BD56" s="26"/>
       <c r="BE56" t="s" s="16">
         <v>851</v>
@@ -15779,7 +15750,7 @@
       </c>
     </row>
     <row r="57" ht="17" customHeight="1">
-      <c r="A57" s="29"/>
+      <c r="A57" s="28"/>
       <c r="B57" t="s" s="14">
         <v>136</v>
       </c>
@@ -15852,7 +15823,7 @@
       <c r="Y57" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z57" s="30"/>
+      <c r="Z57" s="29"/>
       <c r="AA57" t="s" s="21">
         <v>249</v>
       </c>
@@ -15931,7 +15902,7 @@
       <c r="BB57" t="s" s="14">
         <v>861</v>
       </c>
-      <c r="BC57" s="31"/>
+      <c r="BC57" s="30"/>
       <c r="BD57" s="26"/>
       <c r="BE57" t="s" s="16">
         <v>862</v>
@@ -15946,7 +15917,7 @@
       </c>
     </row>
     <row r="58" ht="17" customHeight="1">
-      <c r="A58" s="29"/>
+      <c r="A58" s="28"/>
       <c r="B58" t="s" s="14">
         <v>136</v>
       </c>
@@ -16019,7 +15990,7 @@
       <c r="Y58" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z58" s="34"/>
+      <c r="Z58" s="33"/>
       <c r="AA58" t="s" s="21">
         <v>158</v>
       </c>
@@ -16098,7 +16069,7 @@
       <c r="BB58" t="s" s="14">
         <v>873</v>
       </c>
-      <c r="BC58" s="31"/>
+      <c r="BC58" s="30"/>
       <c r="BD58" s="26"/>
       <c r="BE58" t="s" s="16">
         <v>874</v>
@@ -16113,7 +16084,7 @@
       </c>
     </row>
     <row r="59" ht="17" customHeight="1">
-      <c r="A59" s="29"/>
+      <c r="A59" s="28"/>
       <c r="B59" t="s" s="14">
         <v>136</v>
       </c>
@@ -16186,7 +16157,7 @@
       <c r="Y59" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z59" s="34"/>
+      <c r="Z59" s="33"/>
       <c r="AA59" t="s" s="21">
         <v>158</v>
       </c>
@@ -16265,7 +16236,7 @@
       <c r="BB59" t="s" s="14">
         <v>885</v>
       </c>
-      <c r="BC59" s="31"/>
+      <c r="BC59" s="30"/>
       <c r="BD59" s="26"/>
       <c r="BE59" t="s" s="16">
         <v>886</v>
@@ -16280,7 +16251,7 @@
       </c>
     </row>
     <row r="60" ht="17" customHeight="1">
-      <c r="A60" s="29"/>
+      <c r="A60" s="28"/>
       <c r="B60" t="s" s="14">
         <v>136</v>
       </c>
@@ -16353,7 +16324,7 @@
       <c r="Y60" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z60" s="34"/>
+      <c r="Z60" s="33"/>
       <c r="AA60" t="s" s="21">
         <v>249</v>
       </c>
@@ -16449,7 +16420,7 @@
       </c>
     </row>
     <row r="61" ht="17" customHeight="1">
-      <c r="A61" s="29"/>
+      <c r="A61" s="28"/>
       <c r="B61" t="s" s="14">
         <v>136</v>
       </c>
@@ -16522,7 +16493,7 @@
       <c r="Y61" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z61" s="30"/>
+      <c r="Z61" s="29"/>
       <c r="AA61" t="s" s="21">
         <v>249</v>
       </c>
@@ -16601,7 +16572,7 @@
       <c r="BB61" t="s" s="14">
         <v>907</v>
       </c>
-      <c r="BC61" s="31"/>
+      <c r="BC61" s="30"/>
       <c r="BD61" s="26"/>
       <c r="BE61" t="s" s="16">
         <v>908</v>
@@ -16616,7 +16587,7 @@
       </c>
     </row>
     <row r="62" ht="17" customHeight="1">
-      <c r="A62" s="29"/>
+      <c r="A62" s="28"/>
       <c r="B62" t="s" s="14">
         <v>136</v>
       </c>
@@ -16689,7 +16660,7 @@
       <c r="Y62" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z62" s="34"/>
+      <c r="Z62" s="33"/>
       <c r="AA62" t="s" s="21">
         <v>292</v>
       </c>
@@ -16768,7 +16739,7 @@
       <c r="BB62" t="s" s="14">
         <v>923</v>
       </c>
-      <c r="BC62" s="31"/>
+      <c r="BC62" s="30"/>
       <c r="BD62" s="26"/>
       <c r="BE62" t="s" s="16">
         <v>924</v>
@@ -16783,7 +16754,7 @@
       </c>
     </row>
     <row r="63" ht="17" customHeight="1">
-      <c r="A63" s="29"/>
+      <c r="A63" s="28"/>
       <c r="B63" t="s" s="14">
         <v>136</v>
       </c>
@@ -16856,7 +16827,7 @@
       <c r="Y63" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z63" s="30"/>
+      <c r="Z63" s="29"/>
       <c r="AA63" t="s" s="21">
         <v>249</v>
       </c>
@@ -16935,7 +16906,7 @@
       <c r="BB63" t="s" s="14">
         <v>936</v>
       </c>
-      <c r="BC63" s="31"/>
+      <c r="BC63" s="30"/>
       <c r="BD63" s="26"/>
       <c r="BE63" t="s" s="16">
         <v>937</v>
@@ -16950,7 +16921,7 @@
       </c>
     </row>
     <row r="64" ht="17" customHeight="1">
-      <c r="A64" s="29"/>
+      <c r="A64" s="28"/>
       <c r="B64" t="s" s="14">
         <v>136</v>
       </c>
@@ -17023,7 +16994,7 @@
       <c r="Y64" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z64" s="30"/>
+      <c r="Z64" s="29"/>
       <c r="AA64" t="s" s="21">
         <v>249</v>
       </c>
@@ -17102,7 +17073,7 @@
       <c r="BB64" t="s" s="14">
         <v>949</v>
       </c>
-      <c r="BC64" s="31"/>
+      <c r="BC64" s="30"/>
       <c r="BD64" s="26"/>
       <c r="BE64" t="s" s="16">
         <v>950</v>
@@ -17117,7 +17088,7 @@
       </c>
     </row>
     <row r="65" ht="17" customHeight="1">
-      <c r="A65" s="29"/>
+      <c r="A65" s="28"/>
       <c r="B65" t="s" s="14">
         <v>136</v>
       </c>
@@ -17190,7 +17161,7 @@
       <c r="Y65" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z65" s="34"/>
+      <c r="Z65" s="33"/>
       <c r="AA65" t="s" s="21">
         <v>249</v>
       </c>
@@ -17269,7 +17240,7 @@
       <c r="BB65" t="s" s="14">
         <v>962</v>
       </c>
-      <c r="BC65" s="31"/>
+      <c r="BC65" s="30"/>
       <c r="BD65" s="26"/>
       <c r="BE65" t="s" s="16">
         <v>963</v>
@@ -17284,7 +17255,7 @@
       </c>
     </row>
     <row r="66" ht="17" customHeight="1">
-      <c r="A66" s="29"/>
+      <c r="A66" s="28"/>
       <c r="B66" t="s" s="14">
         <v>136</v>
       </c>
@@ -17357,7 +17328,7 @@
       <c r="Y66" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z66" s="30"/>
+      <c r="Z66" s="29"/>
       <c r="AA66" t="s" s="21">
         <v>249</v>
       </c>
@@ -17436,7 +17407,7 @@
       <c r="BB66" t="s" s="14">
         <v>973</v>
       </c>
-      <c r="BC66" t="s" s="40">
+      <c r="BC66" t="s" s="39">
         <v>974</v>
       </c>
       <c r="BD66" s="26"/>
@@ -17455,7 +17426,7 @@
       </c>
     </row>
     <row r="67" ht="17" customHeight="1">
-      <c r="A67" s="29"/>
+      <c r="A67" s="28"/>
       <c r="B67" t="s" s="14">
         <v>136</v>
       </c>
@@ -17528,7 +17499,7 @@
       <c r="Y67" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z67" s="30"/>
+      <c r="Z67" s="29"/>
       <c r="AA67" t="s" s="21">
         <v>249</v>
       </c>
@@ -17607,7 +17578,7 @@
       <c r="BB67" t="s" s="14">
         <v>987</v>
       </c>
-      <c r="BC67" s="31"/>
+      <c r="BC67" s="30"/>
       <c r="BD67" s="26"/>
       <c r="BE67" t="s" s="16">
         <v>988</v>
@@ -17622,7 +17593,7 @@
       </c>
     </row>
     <row r="68" ht="17" customHeight="1">
-      <c r="A68" s="29"/>
+      <c r="A68" s="28"/>
       <c r="B68" t="s" s="14">
         <v>136</v>
       </c>
@@ -17695,7 +17666,7 @@
       <c r="Y68" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z68" s="30"/>
+      <c r="Z68" s="29"/>
       <c r="AA68" t="s" s="21">
         <v>158</v>
       </c>
@@ -17791,7 +17762,7 @@
       </c>
     </row>
     <row r="69" ht="17" customHeight="1">
-      <c r="A69" s="29"/>
+      <c r="A69" s="28"/>
       <c r="B69" t="s" s="14">
         <v>136</v>
       </c>
@@ -17864,7 +17835,7 @@
       <c r="Y69" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z69" s="30"/>
+      <c r="Z69" s="29"/>
       <c r="AA69" t="s" s="21">
         <v>158</v>
       </c>
@@ -17943,7 +17914,7 @@
       <c r="BB69" t="s" s="14">
         <v>1012</v>
       </c>
-      <c r="BC69" s="31"/>
+      <c r="BC69" s="30"/>
       <c r="BD69" s="26"/>
       <c r="BE69" t="s" s="16">
         <v>1013</v>
@@ -17958,7 +17929,7 @@
       </c>
     </row>
     <row r="70" ht="17" customHeight="1">
-      <c r="A70" s="29"/>
+      <c r="A70" s="28"/>
       <c r="B70" t="s" s="14">
         <v>136</v>
       </c>
@@ -18031,7 +18002,7 @@
       <c r="Y70" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z70" s="34"/>
+      <c r="Z70" s="33"/>
       <c r="AA70" t="s" s="21">
         <v>249</v>
       </c>
@@ -18110,7 +18081,7 @@
       <c r="BB70" t="s" s="14">
         <v>1027</v>
       </c>
-      <c r="BC70" t="s" s="40">
+      <c r="BC70" t="s" s="39">
         <v>1028</v>
       </c>
       <c r="BD70" s="26"/>
@@ -18127,7 +18098,7 @@
       </c>
     </row>
     <row r="71" ht="17" customHeight="1">
-      <c r="A71" s="29"/>
+      <c r="A71" s="28"/>
       <c r="B71" t="s" s="14">
         <v>136</v>
       </c>
@@ -18200,7 +18171,7 @@
       <c r="Y71" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z71" s="34"/>
+      <c r="Z71" s="33"/>
       <c r="AA71" t="s" s="21">
         <v>249</v>
       </c>
@@ -18279,7 +18250,7 @@
       <c r="BB71" t="s" s="14">
         <v>1041</v>
       </c>
-      <c r="BC71" t="s" s="40">
+      <c r="BC71" t="s" s="39">
         <v>1042</v>
       </c>
       <c r="BD71" s="26"/>
@@ -18296,7 +18267,7 @@
       </c>
     </row>
     <row r="72" ht="17" customHeight="1">
-      <c r="A72" s="29"/>
+      <c r="A72" s="28"/>
       <c r="B72" t="s" s="14">
         <v>136</v>
       </c>
@@ -18369,7 +18340,7 @@
       <c r="Y72" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z72" s="30"/>
+      <c r="Z72" s="29"/>
       <c r="AA72" t="s" s="21">
         <v>249</v>
       </c>
@@ -18448,7 +18419,7 @@
       <c r="BB72" t="s" s="14">
         <v>1052</v>
       </c>
-      <c r="BC72" t="s" s="40">
+      <c r="BC72" t="s" s="39">
         <v>1053</v>
       </c>
       <c r="BD72" s="26"/>
@@ -18465,7 +18436,7 @@
       </c>
     </row>
     <row r="73" ht="17" customHeight="1">
-      <c r="A73" s="29"/>
+      <c r="A73" s="28"/>
       <c r="B73" t="s" s="14">
         <v>136</v>
       </c>
@@ -18484,10 +18455,10 @@
       <c r="G73" t="s" s="16">
         <v>1032</v>
       </c>
-      <c r="H73" t="s" s="32">
+      <c r="H73" t="s" s="31">
         <v>1057</v>
       </c>
-      <c r="I73" t="s" s="33">
+      <c r="I73" t="s" s="32">
         <v>1058</v>
       </c>
       <c r="J73" t="s" s="18">
@@ -18538,7 +18509,7 @@
       <c r="Y73" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z73" s="34"/>
+      <c r="Z73" s="33"/>
       <c r="AA73" t="s" s="21">
         <v>249</v>
       </c>
@@ -18617,7 +18588,7 @@
       <c r="BB73" t="s" s="14">
         <v>1066</v>
       </c>
-      <c r="BC73" t="s" s="40">
+      <c r="BC73" t="s" s="39">
         <v>1067</v>
       </c>
       <c r="BD73" s="26"/>
@@ -18634,7 +18605,7 @@
       </c>
     </row>
     <row r="74" ht="17" customHeight="1">
-      <c r="A74" s="29"/>
+      <c r="A74" s="28"/>
       <c r="B74" t="s" s="14">
         <v>136</v>
       </c>
@@ -18707,7 +18678,7 @@
       <c r="Y74" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z74" s="30"/>
+      <c r="Z74" s="29"/>
       <c r="AA74" t="s" s="21">
         <v>249</v>
       </c>
@@ -18786,7 +18757,7 @@
       <c r="BB74" t="s" s="14">
         <v>1077</v>
       </c>
-      <c r="BC74" s="31"/>
+      <c r="BC74" s="30"/>
       <c r="BD74" s="26"/>
       <c r="BE74" t="s" s="16">
         <v>1078</v>
@@ -18801,7 +18772,7 @@
       </c>
     </row>
     <row r="75" ht="17" customHeight="1">
-      <c r="A75" s="29"/>
+      <c r="A75" s="28"/>
       <c r="B75" t="s" s="14">
         <v>136</v>
       </c>
@@ -18874,7 +18845,7 @@
       <c r="Y75" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z75" s="34"/>
+      <c r="Z75" s="33"/>
       <c r="AA75" t="s" s="21">
         <v>249</v>
       </c>
@@ -18953,7 +18924,7 @@
       <c r="BB75" t="s" s="14">
         <v>1091</v>
       </c>
-      <c r="BC75" s="31"/>
+      <c r="BC75" s="30"/>
       <c r="BD75" s="26"/>
       <c r="BE75" t="s" s="16">
         <v>1092</v>
@@ -18968,7 +18939,7 @@
       </c>
     </row>
     <row r="76" ht="17" customHeight="1">
-      <c r="A76" s="29"/>
+      <c r="A76" s="28"/>
       <c r="B76" t="s" s="14">
         <v>136</v>
       </c>
@@ -19041,7 +19012,7 @@
       <c r="Y76" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z76" s="34"/>
+      <c r="Z76" s="33"/>
       <c r="AA76" t="s" s="21">
         <v>249</v>
       </c>
@@ -19120,7 +19091,7 @@
       <c r="BB76" t="s" s="14">
         <v>1103</v>
       </c>
-      <c r="BC76" t="s" s="40">
+      <c r="BC76" t="s" s="39">
         <v>208</v>
       </c>
       <c r="BD76" s="26"/>
@@ -19137,7 +19108,7 @@
       </c>
     </row>
     <row r="77" ht="17" customHeight="1">
-      <c r="A77" s="29"/>
+      <c r="A77" s="28"/>
       <c r="B77" t="s" s="14">
         <v>136</v>
       </c>
@@ -19210,7 +19181,7 @@
       <c r="Y77" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z77" s="34"/>
+      <c r="Z77" s="33"/>
       <c r="AA77" t="s" s="21">
         <v>249</v>
       </c>
@@ -19289,7 +19260,7 @@
       <c r="BB77" t="s" s="14">
         <v>1114</v>
       </c>
-      <c r="BC77" s="31"/>
+      <c r="BC77" s="30"/>
       <c r="BD77" s="26"/>
       <c r="BE77" t="s" s="16">
         <v>1115</v>
@@ -19304,7 +19275,7 @@
       </c>
     </row>
     <row r="78" ht="17" customHeight="1">
-      <c r="A78" s="29"/>
+      <c r="A78" s="28"/>
       <c r="B78" t="s" s="14">
         <v>136</v>
       </c>
@@ -19377,7 +19348,7 @@
       <c r="Y78" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z78" s="30"/>
+      <c r="Z78" s="29"/>
       <c r="AA78" t="s" s="21">
         <v>249</v>
       </c>
@@ -19456,7 +19427,7 @@
       <c r="BB78" t="s" s="14">
         <v>1126</v>
       </c>
-      <c r="BC78" t="s" s="40">
+      <c r="BC78" t="s" s="39">
         <v>401</v>
       </c>
       <c r="BD78" s="26"/>
@@ -19473,7 +19444,7 @@
       </c>
     </row>
     <row r="79" ht="17" customHeight="1">
-      <c r="A79" s="29"/>
+      <c r="A79" s="28"/>
       <c r="B79" t="s" s="14">
         <v>136</v>
       </c>
@@ -19546,7 +19517,7 @@
       <c r="Y79" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z79" s="30"/>
+      <c r="Z79" s="29"/>
       <c r="AA79" t="s" s="21">
         <v>249</v>
       </c>
@@ -19625,7 +19596,7 @@
       <c r="BB79" t="s" s="14">
         <v>1135</v>
       </c>
-      <c r="BC79" t="s" s="40">
+      <c r="BC79" t="s" s="39">
         <v>1136</v>
       </c>
       <c r="BD79" s="26"/>
@@ -19642,7 +19613,7 @@
       </c>
     </row>
     <row r="80" ht="17" customHeight="1">
-      <c r="A80" s="29"/>
+      <c r="A80" s="28"/>
       <c r="B80" t="s" s="14">
         <v>136</v>
       </c>
@@ -19715,7 +19686,7 @@
       <c r="Y80" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z80" s="30"/>
+      <c r="Z80" s="29"/>
       <c r="AA80" t="s" s="21">
         <v>249</v>
       </c>
@@ -19794,7 +19765,7 @@
       <c r="BB80" t="s" s="14">
         <v>1147</v>
       </c>
-      <c r="BC80" t="s" s="40">
+      <c r="BC80" t="s" s="39">
         <v>1148</v>
       </c>
       <c r="BD80" s="26"/>
@@ -19811,7 +19782,7 @@
       </c>
     </row>
     <row r="81" ht="17" customHeight="1">
-      <c r="A81" s="29"/>
+      <c r="A81" s="28"/>
       <c r="B81" t="s" s="14">
         <v>136</v>
       </c>
@@ -19884,7 +19855,7 @@
       <c r="Y81" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z81" s="34"/>
+      <c r="Z81" s="33"/>
       <c r="AA81" t="s" s="21">
         <v>249</v>
       </c>
@@ -19963,7 +19934,7 @@
       <c r="BB81" t="s" s="14">
         <v>1158</v>
       </c>
-      <c r="BC81" t="s" s="40">
+      <c r="BC81" t="s" s="39">
         <v>1159</v>
       </c>
       <c r="BD81" s="26"/>
@@ -19980,7 +19951,7 @@
       </c>
     </row>
     <row r="82" ht="17" customHeight="1">
-      <c r="A82" s="29"/>
+      <c r="A82" s="28"/>
       <c r="B82" t="s" s="14">
         <v>136</v>
       </c>
@@ -20053,7 +20024,7 @@
       <c r="Y82" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z82" s="30"/>
+      <c r="Z82" s="29"/>
       <c r="AA82" t="s" s="21">
         <v>249</v>
       </c>
@@ -20132,7 +20103,7 @@
       <c r="BB82" t="s" s="14">
         <v>1170</v>
       </c>
-      <c r="BC82" s="31"/>
+      <c r="BC82" s="30"/>
       <c r="BD82" s="26"/>
       <c r="BE82" t="s" s="16">
         <v>1171</v>
@@ -20147,7 +20118,7 @@
       </c>
     </row>
     <row r="83" ht="17" customHeight="1">
-      <c r="A83" s="29"/>
+      <c r="A83" s="28"/>
       <c r="B83" t="s" s="14">
         <v>136</v>
       </c>
@@ -20220,7 +20191,7 @@
       <c r="Y83" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z83" s="30"/>
+      <c r="Z83" s="29"/>
       <c r="AA83" t="s" s="21">
         <v>249</v>
       </c>
@@ -20299,7 +20270,7 @@
       <c r="BB83" t="s" s="14">
         <v>1181</v>
       </c>
-      <c r="BC83" s="31"/>
+      <c r="BC83" s="30"/>
       <c r="BD83" s="26"/>
       <c r="BE83" t="s" s="16">
         <v>1182</v>
@@ -20314,7 +20285,7 @@
       </c>
     </row>
     <row r="84" ht="17" customHeight="1">
-      <c r="A84" s="29"/>
+      <c r="A84" s="28"/>
       <c r="B84" t="s" s="14">
         <v>136</v>
       </c>
@@ -20387,7 +20358,7 @@
       <c r="Y84" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z84" s="34"/>
+      <c r="Z84" s="33"/>
       <c r="AA84" t="s" s="21">
         <v>249</v>
       </c>
@@ -20466,7 +20437,7 @@
       <c r="BB84" t="s" s="14">
         <v>1194</v>
       </c>
-      <c r="BC84" s="31"/>
+      <c r="BC84" s="30"/>
       <c r="BD84" s="26"/>
       <c r="BE84" t="s" s="16">
         <v>1195</v>
@@ -20481,7 +20452,7 @@
       </c>
     </row>
     <row r="85" ht="17" customHeight="1">
-      <c r="A85" s="29"/>
+      <c r="A85" s="28"/>
       <c r="B85" t="s" s="14">
         <v>136</v>
       </c>
@@ -20554,7 +20525,7 @@
       <c r="Y85" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z85" s="30"/>
+      <c r="Z85" s="29"/>
       <c r="AA85" t="s" s="21">
         <v>292</v>
       </c>
@@ -20633,7 +20604,7 @@
       <c r="BB85" t="s" s="14">
         <v>1207</v>
       </c>
-      <c r="BC85" t="s" s="40">
+      <c r="BC85" t="s" s="39">
         <v>1208</v>
       </c>
       <c r="BD85" s="26"/>
@@ -20650,7 +20621,7 @@
       </c>
     </row>
     <row r="86" ht="17" customHeight="1">
-      <c r="A86" s="29"/>
+      <c r="A86" s="28"/>
       <c r="B86" t="s" s="14">
         <v>136</v>
       </c>
@@ -20723,7 +20694,7 @@
       <c r="Y86" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z86" s="34"/>
+      <c r="Z86" s="33"/>
       <c r="AA86" t="s" s="21">
         <v>249</v>
       </c>
@@ -20802,7 +20773,7 @@
       <c r="BB86" t="s" s="14">
         <v>1220</v>
       </c>
-      <c r="BC86" t="s" s="40">
+      <c r="BC86" t="s" s="39">
         <v>401</v>
       </c>
       <c r="BD86" s="26"/>
@@ -20819,7 +20790,7 @@
       </c>
     </row>
     <row r="87" ht="17" customHeight="1">
-      <c r="A87" s="29"/>
+      <c r="A87" s="28"/>
       <c r="B87" t="s" s="14">
         <v>136</v>
       </c>
@@ -20892,7 +20863,7 @@
       <c r="Y87" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z87" s="30"/>
+      <c r="Z87" s="29"/>
       <c r="AA87" t="s" s="21">
         <v>158</v>
       </c>
@@ -20963,11 +20934,11 @@
       <c r="AZ87" t="s" s="14">
         <v>1232</v>
       </c>
-      <c r="BA87" s="41"/>
+      <c r="BA87" s="40"/>
       <c r="BB87" t="s" s="14">
         <v>1233</v>
       </c>
-      <c r="BC87" t="s" s="40">
+      <c r="BC87" t="s" s="39">
         <v>1234</v>
       </c>
       <c r="BD87" s="26"/>
@@ -20986,7 +20957,7 @@
       </c>
     </row>
     <row r="88" ht="17" customHeight="1">
-      <c r="A88" s="29"/>
+      <c r="A88" s="28"/>
       <c r="B88" t="s" s="14">
         <v>136</v>
       </c>
@@ -21059,7 +21030,7 @@
       <c r="Y88" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z88" s="30"/>
+      <c r="Z88" s="29"/>
       <c r="AA88" t="s" s="21">
         <v>192</v>
       </c>
@@ -21138,7 +21109,7 @@
       <c r="BB88" t="s" s="14">
         <v>1246</v>
       </c>
-      <c r="BC88" t="s" s="40">
+      <c r="BC88" t="s" s="39">
         <v>1247</v>
       </c>
       <c r="BD88" s="26"/>
@@ -21157,7 +21128,7 @@
       </c>
     </row>
     <row r="89" ht="17" customHeight="1">
-      <c r="A89" s="29"/>
+      <c r="A89" s="28"/>
       <c r="B89" t="s" s="14">
         <v>136</v>
       </c>
@@ -21230,7 +21201,7 @@
       <c r="Y89" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z89" s="30"/>
+      <c r="Z89" s="29"/>
       <c r="AA89" t="s" s="21">
         <v>249</v>
       </c>
@@ -21309,7 +21280,7 @@
       <c r="BB89" t="s" s="14">
         <v>1261</v>
       </c>
-      <c r="BC89" t="s" s="40">
+      <c r="BC89" t="s" s="39">
         <v>401</v>
       </c>
       <c r="BD89" s="26"/>
@@ -21326,7 +21297,7 @@
       </c>
     </row>
     <row r="90" ht="17" customHeight="1">
-      <c r="A90" s="29"/>
+      <c r="A90" s="28"/>
       <c r="B90" t="s" s="14">
         <v>136</v>
       </c>
@@ -21399,7 +21370,7 @@
       <c r="Y90" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z90" s="30"/>
+      <c r="Z90" s="29"/>
       <c r="AA90" t="s" s="21">
         <v>249</v>
       </c>
@@ -21478,7 +21449,7 @@
       <c r="BB90" t="s" s="14">
         <v>1275</v>
       </c>
-      <c r="BC90" t="s" s="40">
+      <c r="BC90" t="s" s="39">
         <v>401</v>
       </c>
       <c r="BD90" s="26"/>
@@ -21495,7 +21466,7 @@
       </c>
     </row>
     <row r="91" ht="17" customHeight="1">
-      <c r="A91" s="29"/>
+      <c r="A91" s="28"/>
       <c r="B91" t="s" s="14">
         <v>136</v>
       </c>
@@ -21568,7 +21539,7 @@
       <c r="Y91" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z91" s="30"/>
+      <c r="Z91" s="29"/>
       <c r="AA91" t="s" s="21">
         <v>292</v>
       </c>
@@ -21647,7 +21618,7 @@
       <c r="BB91" t="s" s="14">
         <v>1286</v>
       </c>
-      <c r="BC91" s="31"/>
+      <c r="BC91" s="30"/>
       <c r="BD91" s="26"/>
       <c r="BE91" t="s" s="16">
         <v>1287</v>
@@ -21662,7 +21633,7 @@
       </c>
     </row>
     <row r="92" ht="17" customHeight="1">
-      <c r="A92" s="29"/>
+      <c r="A92" s="28"/>
       <c r="B92" t="s" s="14">
         <v>136</v>
       </c>
@@ -21735,7 +21706,7 @@
       <c r="Y92" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z92" s="30"/>
+      <c r="Z92" s="29"/>
       <c r="AA92" t="s" s="21">
         <v>249</v>
       </c>
@@ -21814,7 +21785,7 @@
       <c r="BB92" t="s" s="14">
         <v>1297</v>
       </c>
-      <c r="BC92" s="31"/>
+      <c r="BC92" s="30"/>
       <c r="BD92" s="26"/>
       <c r="BE92" t="s" s="16">
         <v>1298</v>
@@ -21829,7 +21800,7 @@
       </c>
     </row>
     <row r="93" ht="17" customHeight="1">
-      <c r="A93" s="29"/>
+      <c r="A93" s="28"/>
       <c r="B93" t="s" s="14">
         <v>136</v>
       </c>
@@ -21902,7 +21873,7 @@
       <c r="Y93" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z93" s="30"/>
+      <c r="Z93" s="29"/>
       <c r="AA93" t="s" s="21">
         <v>249</v>
       </c>
@@ -21981,7 +21952,7 @@
       <c r="BB93" t="s" s="14">
         <v>1309</v>
       </c>
-      <c r="BC93" s="31"/>
+      <c r="BC93" s="30"/>
       <c r="BD93" s="26"/>
       <c r="BE93" t="s" s="16">
         <v>1310</v>
@@ -21996,7 +21967,7 @@
       </c>
     </row>
     <row r="94" ht="17" customHeight="1">
-      <c r="A94" s="29"/>
+      <c r="A94" s="28"/>
       <c r="B94" t="s" s="14">
         <v>136</v>
       </c>
@@ -22069,7 +22040,7 @@
       <c r="Y94" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z94" s="30"/>
+      <c r="Z94" s="29"/>
       <c r="AA94" t="s" s="21">
         <v>249</v>
       </c>
@@ -22148,7 +22119,7 @@
       <c r="BB94" t="s" s="14">
         <v>1320</v>
       </c>
-      <c r="BC94" s="31"/>
+      <c r="BC94" s="30"/>
       <c r="BD94" s="26"/>
       <c r="BE94" t="s" s="16">
         <v>1321</v>
@@ -22163,7 +22134,7 @@
       </c>
     </row>
     <row r="95" ht="17" customHeight="1">
-      <c r="A95" s="29"/>
+      <c r="A95" s="28"/>
       <c r="B95" t="s" s="14">
         <v>136</v>
       </c>
@@ -22236,7 +22207,7 @@
       <c r="Y95" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z95" s="30"/>
+      <c r="Z95" s="29"/>
       <c r="AA95" t="s" s="21">
         <v>249</v>
       </c>
@@ -22315,7 +22286,7 @@
       <c r="BB95" t="s" s="14">
         <v>1332</v>
       </c>
-      <c r="BC95" t="s" s="40">
+      <c r="BC95" t="s" s="39">
         <v>469</v>
       </c>
       <c r="BD95" s="26"/>
@@ -22332,7 +22303,7 @@
       </c>
     </row>
     <row r="96" ht="17" customHeight="1">
-      <c r="A96" s="29"/>
+      <c r="A96" s="28"/>
       <c r="B96" t="s" s="14">
         <v>136</v>
       </c>
@@ -22405,7 +22376,7 @@
       <c r="Y96" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z96" s="30"/>
+      <c r="Z96" s="29"/>
       <c r="AA96" t="s" s="21">
         <v>192</v>
       </c>
@@ -22484,7 +22455,7 @@
       <c r="BB96" t="s" s="14">
         <v>1342</v>
       </c>
-      <c r="BC96" t="s" s="40">
+      <c r="BC96" t="s" s="39">
         <v>1343</v>
       </c>
       <c r="BD96" s="26"/>
@@ -22501,7 +22472,7 @@
       </c>
     </row>
     <row r="97" ht="17" customHeight="1">
-      <c r="A97" s="29"/>
+      <c r="A97" s="28"/>
       <c r="B97" t="s" s="14">
         <v>136</v>
       </c>
@@ -22574,7 +22545,7 @@
       <c r="Y97" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z97" s="30"/>
+      <c r="Z97" s="29"/>
       <c r="AA97" t="s" s="21">
         <v>192</v>
       </c>
@@ -22653,7 +22624,7 @@
       <c r="BB97" t="s" s="14">
         <v>1354</v>
       </c>
-      <c r="BC97" s="31"/>
+      <c r="BC97" s="30"/>
       <c r="BD97" s="26"/>
       <c r="BE97" t="s" s="16">
         <v>1355</v>
@@ -22668,7 +22639,7 @@
       </c>
     </row>
     <row r="98" ht="17" customHeight="1">
-      <c r="A98" s="29"/>
+      <c r="A98" s="28"/>
       <c r="B98" t="s" s="14">
         <v>136</v>
       </c>
@@ -22741,7 +22712,7 @@
       <c r="Y98" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z98" s="30"/>
+      <c r="Z98" s="29"/>
       <c r="AA98" t="s" s="21">
         <v>158</v>
       </c>
@@ -22837,7 +22808,7 @@
       </c>
     </row>
     <row r="99" ht="17" customHeight="1">
-      <c r="A99" s="29"/>
+      <c r="A99" s="28"/>
       <c r="B99" t="s" s="14">
         <v>136</v>
       </c>
@@ -22910,7 +22881,7 @@
       <c r="Y99" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z99" s="30"/>
+      <c r="Z99" s="29"/>
       <c r="AA99" t="s" s="21">
         <v>249</v>
       </c>
@@ -22989,7 +22960,7 @@
       <c r="BB99" t="s" s="14">
         <v>1378</v>
       </c>
-      <c r="BC99" t="s" s="40">
+      <c r="BC99" t="s" s="39">
         <v>1379</v>
       </c>
       <c r="BD99" s="26"/>
@@ -23006,7 +22977,7 @@
       </c>
     </row>
     <row r="100" ht="17" customHeight="1">
-      <c r="A100" s="29"/>
+      <c r="A100" s="28"/>
       <c r="B100" t="s" s="14">
         <v>136</v>
       </c>
@@ -23025,10 +22996,10 @@
       <c r="G100" t="s" s="16">
         <v>1358</v>
       </c>
-      <c r="H100" t="s" s="32">
+      <c r="H100" t="s" s="31">
         <v>1383</v>
       </c>
-      <c r="I100" t="s" s="33">
+      <c r="I100" t="s" s="32">
         <v>1384</v>
       </c>
       <c r="J100" t="s" s="18">
@@ -23079,7 +23050,7 @@
       <c r="Y100" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z100" s="34"/>
+      <c r="Z100" s="33"/>
       <c r="AA100" t="s" s="21">
         <v>249</v>
       </c>
@@ -23158,7 +23129,7 @@
       <c r="BB100" t="s" s="14">
         <v>1389</v>
       </c>
-      <c r="BC100" t="s" s="40">
+      <c r="BC100" t="s" s="39">
         <v>208</v>
       </c>
       <c r="BD100" s="26"/>
@@ -23175,7 +23146,7 @@
       </c>
     </row>
     <row r="101" ht="17" customHeight="1">
-      <c r="A101" s="29"/>
+      <c r="A101" s="28"/>
       <c r="B101" t="s" s="14">
         <v>136</v>
       </c>
@@ -23194,10 +23165,10 @@
       <c r="G101" t="s" s="16">
         <v>1358</v>
       </c>
-      <c r="H101" t="s" s="32">
+      <c r="H101" t="s" s="31">
         <v>1393</v>
       </c>
-      <c r="I101" t="s" s="33">
+      <c r="I101" t="s" s="32">
         <v>246</v>
       </c>
       <c r="J101" t="s" s="18">
@@ -23248,7 +23219,7 @@
       <c r="Y101" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z101" s="34"/>
+      <c r="Z101" s="33"/>
       <c r="AA101" t="s" s="21">
         <v>292</v>
       </c>
@@ -23327,7 +23298,7 @@
       <c r="BB101" t="s" s="14">
         <v>1399</v>
       </c>
-      <c r="BC101" t="s" s="40">
+      <c r="BC101" t="s" s="39">
         <v>717</v>
       </c>
       <c r="BD101" s="26"/>
@@ -23344,7 +23315,7 @@
       </c>
     </row>
     <row r="102" ht="17" customHeight="1">
-      <c r="A102" s="29"/>
+      <c r="A102" s="28"/>
       <c r="B102" t="s" s="14">
         <v>136</v>
       </c>
@@ -23417,7 +23388,7 @@
       <c r="Y102" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z102" s="30"/>
+      <c r="Z102" s="29"/>
       <c r="AA102" t="s" s="21">
         <v>249</v>
       </c>
@@ -23496,7 +23467,7 @@
       <c r="BB102" t="s" s="14">
         <v>1413</v>
       </c>
-      <c r="BC102" t="s" s="40">
+      <c r="BC102" t="s" s="39">
         <v>401</v>
       </c>
       <c r="BD102" s="26"/>
@@ -23513,7 +23484,7 @@
       </c>
     </row>
     <row r="103" ht="17" customHeight="1">
-      <c r="A103" s="29"/>
+      <c r="A103" s="28"/>
       <c r="B103" t="s" s="14">
         <v>136</v>
       </c>
@@ -23586,7 +23557,7 @@
       <c r="Y103" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z103" s="30"/>
+      <c r="Z103" s="29"/>
       <c r="AA103" t="s" s="21">
         <v>249</v>
       </c>
@@ -23647,7 +23618,7 @@
       <c r="AT103" t="s" s="21">
         <v>199</v>
       </c>
-      <c r="AU103" s="45"/>
+      <c r="AU103" s="43"/>
       <c r="AV103" t="s" s="14">
         <v>1422</v>
       </c>
@@ -23663,7 +23634,7 @@
       <c r="BB103" t="s" s="14">
         <v>1425</v>
       </c>
-      <c r="BC103" s="31"/>
+      <c r="BC103" s="30"/>
       <c r="BD103" s="26"/>
       <c r="BE103" t="s" s="16">
         <v>1426</v>
@@ -23678,7 +23649,7 @@
       </c>
     </row>
     <row r="104" ht="17" customHeight="1">
-      <c r="A104" s="29"/>
+      <c r="A104" s="28"/>
       <c r="B104" t="s" s="14">
         <v>136</v>
       </c>
@@ -23749,7 +23720,7 @@
       <c r="Y104" t="s" s="14">
         <v>156</v>
       </c>
-      <c r="Z104" s="30"/>
+      <c r="Z104" s="29"/>
       <c r="AA104" t="s" s="21">
         <v>292</v>
       </c>
@@ -23828,7 +23799,7 @@
       <c r="BB104" t="s" s="14">
         <v>1436</v>
       </c>
-      <c r="BC104" s="31"/>
+      <c r="BC104" s="30"/>
       <c r="BD104" s="26"/>
       <c r="BE104" t="s" s="16">
         <v>1437</v>
@@ -23845,7 +23816,7 @@
       </c>
     </row>
     <row r="105" ht="17" customHeight="1">
-      <c r="A105" s="46"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="26"/>
       <c r="C105" s="26"/>
       <c r="D105" s="26"/>
@@ -23871,27 +23842,27 @@
       <c r="X105" s="26"/>
       <c r="Y105" s="26"/>
       <c r="Z105" s="26"/>
-      <c r="AA105" s="47"/>
-      <c r="AB105" s="48"/>
-      <c r="AC105" s="48"/>
-      <c r="AD105" s="48"/>
-      <c r="AE105" s="48"/>
-      <c r="AF105" s="48"/>
-      <c r="AG105" s="48"/>
-      <c r="AH105" s="48"/>
-      <c r="AI105" s="48"/>
-      <c r="AJ105" s="48"/>
-      <c r="AK105" s="48"/>
-      <c r="AL105" s="48"/>
-      <c r="AM105" s="48"/>
-      <c r="AN105" s="48"/>
-      <c r="AO105" s="48"/>
-      <c r="AP105" s="48"/>
-      <c r="AQ105" s="48"/>
-      <c r="AR105" s="48"/>
-      <c r="AS105" s="48"/>
-      <c r="AT105" s="48"/>
-      <c r="AU105" s="49"/>
+      <c r="AA105" s="45"/>
+      <c r="AB105" s="46"/>
+      <c r="AC105" s="46"/>
+      <c r="AD105" s="46"/>
+      <c r="AE105" s="46"/>
+      <c r="AF105" s="46"/>
+      <c r="AG105" s="46"/>
+      <c r="AH105" s="46"/>
+      <c r="AI105" s="46"/>
+      <c r="AJ105" s="46"/>
+      <c r="AK105" s="46"/>
+      <c r="AL105" s="46"/>
+      <c r="AM105" s="46"/>
+      <c r="AN105" s="46"/>
+      <c r="AO105" s="46"/>
+      <c r="AP105" s="46"/>
+      <c r="AQ105" s="46"/>
+      <c r="AR105" s="46"/>
+      <c r="AS105" s="46"/>
+      <c r="AT105" s="46"/>
+      <c r="AU105" s="47"/>
       <c r="AV105" s="26"/>
       <c r="AW105" s="26"/>
       <c r="AX105" s="26"/>
@@ -23908,7 +23879,7 @@
       <c r="BI105" s="26"/>
     </row>
     <row r="106" ht="17" customHeight="1">
-      <c r="A106" s="46"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="26"/>
       <c r="C106" s="26"/>
       <c r="D106" s="26"/>
@@ -23934,29 +23905,29 @@
       <c r="X106" s="26"/>
       <c r="Y106" s="26"/>
       <c r="Z106" s="26"/>
-      <c r="AA106" t="s" s="51">
+      <c r="AA106" t="s" s="48">
         <v>1441</v>
       </c>
-      <c r="AB106" s="52"/>
-      <c r="AC106" s="52"/>
-      <c r="AD106" s="52"/>
-      <c r="AE106" s="52"/>
-      <c r="AF106" s="52"/>
-      <c r="AG106" s="52"/>
-      <c r="AH106" s="52"/>
-      <c r="AI106" s="52"/>
-      <c r="AJ106" s="52"/>
-      <c r="AK106" s="52"/>
-      <c r="AL106" s="52"/>
-      <c r="AM106" s="52"/>
-      <c r="AN106" s="52"/>
-      <c r="AO106" s="52"/>
-      <c r="AP106" s="52"/>
-      <c r="AQ106" s="52"/>
-      <c r="AR106" s="52"/>
-      <c r="AS106" s="52"/>
-      <c r="AT106" s="52"/>
-      <c r="AU106" s="53"/>
+      <c r="AB106" s="49"/>
+      <c r="AC106" s="49"/>
+      <c r="AD106" s="49"/>
+      <c r="AE106" s="49"/>
+      <c r="AF106" s="49"/>
+      <c r="AG106" s="49"/>
+      <c r="AH106" s="49"/>
+      <c r="AI106" s="49"/>
+      <c r="AJ106" s="49"/>
+      <c r="AK106" s="49"/>
+      <c r="AL106" s="49"/>
+      <c r="AM106" s="49"/>
+      <c r="AN106" s="49"/>
+      <c r="AO106" s="49"/>
+      <c r="AP106" s="49"/>
+      <c r="AQ106" s="49"/>
+      <c r="AR106" s="49"/>
+      <c r="AS106" s="49"/>
+      <c r="AT106" s="49"/>
+      <c r="AU106" s="50"/>
       <c r="AV106" s="26"/>
       <c r="AW106" s="26"/>
       <c r="AX106" s="26"/>
@@ -23973,7 +23944,7 @@
       <c r="BI106" s="26"/>
     </row>
     <row r="107" ht="17" customHeight="1">
-      <c r="A107" s="46"/>
+      <c r="A107" s="44"/>
       <c r="B107" s="26"/>
       <c r="C107" s="26"/>
       <c r="D107" s="26"/>
@@ -24036,7 +24007,7 @@
       <c r="BI107" s="26"/>
     </row>
     <row r="108" ht="17" customHeight="1">
-      <c r="A108" s="46"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="26"/>
       <c r="C108" s="26"/>
       <c r="D108" s="26"/>
@@ -24099,7 +24070,7 @@
       <c r="BI108" s="26"/>
     </row>
     <row r="109" ht="17" customHeight="1">
-      <c r="A109" s="46"/>
+      <c r="A109" s="44"/>
       <c r="B109" s="26"/>
       <c r="C109" s="26"/>
       <c r="D109" s="26"/>
@@ -24162,7 +24133,7 @@
       <c r="BI109" s="26"/>
     </row>
     <row r="110" ht="17" customHeight="1">
-      <c r="A110" s="46"/>
+      <c r="A110" s="44"/>
       <c r="B110" s="26"/>
       <c r="C110" s="26"/>
       <c r="D110" s="26"/>
@@ -24225,7 +24196,7 @@
       <c r="BI110" s="26"/>
     </row>
     <row r="111" ht="17" customHeight="1">
-      <c r="A111" s="46"/>
+      <c r="A111" s="44"/>
       <c r="B111" s="26"/>
       <c r="C111" s="26"/>
       <c r="D111" s="26"/>
@@ -24288,7 +24259,7 @@
       <c r="BI111" s="26"/>
     </row>
     <row r="112" ht="17" customHeight="1">
-      <c r="A112" s="46"/>
+      <c r="A112" s="44"/>
       <c r="B112" s="26"/>
       <c r="C112" s="26"/>
       <c r="D112" s="26"/>
@@ -24351,7 +24322,7 @@
       <c r="BI112" s="26"/>
     </row>
     <row r="113" ht="17" customHeight="1">
-      <c r="A113" s="46"/>
+      <c r="A113" s="44"/>
       <c r="B113" s="26"/>
       <c r="C113" s="26"/>
       <c r="D113" s="26"/>
@@ -24414,7 +24385,7 @@
       <c r="BI113" s="26"/>
     </row>
     <row r="114" ht="17" customHeight="1">
-      <c r="A114" s="46"/>
+      <c r="A114" s="44"/>
       <c r="B114" s="26"/>
       <c r="C114" s="26"/>
       <c r="D114" s="26"/>
@@ -24477,7 +24448,7 @@
       <c r="BI114" s="26"/>
     </row>
     <row r="115" ht="17" customHeight="1">
-      <c r="A115" s="46"/>
+      <c r="A115" s="44"/>
       <c r="B115" s="26"/>
       <c r="C115" s="26"/>
       <c r="D115" s="26"/>
@@ -24540,7 +24511,7 @@
       <c r="BI115" s="26"/>
     </row>
     <row r="116" ht="17" customHeight="1">
-      <c r="A116" s="46"/>
+      <c r="A116" s="44"/>
       <c r="B116" s="26"/>
       <c r="C116" s="26"/>
       <c r="D116" s="26"/>
@@ -24603,7 +24574,7 @@
       <c r="BI116" s="26"/>
     </row>
     <row r="117" ht="17" customHeight="1">
-      <c r="A117" s="46"/>
+      <c r="A117" s="44"/>
       <c r="B117" s="26"/>
       <c r="C117" s="26"/>
       <c r="D117" s="26"/>
@@ -24666,7 +24637,7 @@
       <c r="BI117" s="26"/>
     </row>
     <row r="118" ht="17" customHeight="1">
-      <c r="A118" s="46"/>
+      <c r="A118" s="44"/>
       <c r="B118" s="26"/>
       <c r="C118" s="26"/>
       <c r="D118" s="26"/>
@@ -24729,7 +24700,7 @@
       <c r="BI118" s="26"/>
     </row>
     <row r="119" ht="17" customHeight="1">
-      <c r="A119" s="46"/>
+      <c r="A119" s="44"/>
       <c r="B119" s="26"/>
       <c r="C119" s="26"/>
       <c r="D119" s="26"/>
@@ -24792,7 +24763,7 @@
       <c r="BI119" s="26"/>
     </row>
     <row r="120" ht="17" customHeight="1">
-      <c r="A120" s="46"/>
+      <c r="A120" s="44"/>
       <c r="B120" s="26"/>
       <c r="C120" s="26"/>
       <c r="D120" s="26"/>
@@ -24855,7 +24826,7 @@
       <c r="BI120" s="26"/>
     </row>
     <row r="121" ht="17" customHeight="1">
-      <c r="A121" s="46"/>
+      <c r="A121" s="44"/>
       <c r="B121" s="26"/>
       <c r="C121" s="26"/>
       <c r="D121" s="26"/>
@@ -24918,7 +24889,7 @@
       <c r="BI121" s="26"/>
     </row>
     <row r="122" ht="17" customHeight="1">
-      <c r="A122" s="46"/>
+      <c r="A122" s="44"/>
       <c r="B122" s="26"/>
       <c r="C122" s="26"/>
       <c r="D122" s="26"/>
@@ -24981,7 +24952,7 @@
       <c r="BI122" s="26"/>
     </row>
     <row r="123" ht="17" customHeight="1">
-      <c r="A123" s="46"/>
+      <c r="A123" s="44"/>
       <c r="B123" s="26"/>
       <c r="C123" s="26"/>
       <c r="D123" s="26"/>
@@ -25044,7 +25015,7 @@
       <c r="BI123" s="26"/>
     </row>
     <row r="124" ht="17" customHeight="1">
-      <c r="A124" s="46"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="26"/>
       <c r="C124" s="26"/>
       <c r="D124" s="26"/>
@@ -25107,7 +25078,7 @@
       <c r="BI124" s="26"/>
     </row>
     <row r="125" ht="17" customHeight="1">
-      <c r="A125" s="46"/>
+      <c r="A125" s="44"/>
       <c r="B125" s="26"/>
       <c r="C125" s="26"/>
       <c r="D125" s="26"/>
@@ -25170,7 +25141,7 @@
       <c r="BI125" s="26"/>
     </row>
     <row r="126" ht="17" customHeight="1">
-      <c r="A126" s="46"/>
+      <c r="A126" s="44"/>
       <c r="B126" s="26"/>
       <c r="C126" s="26"/>
       <c r="D126" s="26"/>
@@ -25233,7 +25204,7 @@
       <c r="BI126" s="26"/>
     </row>
     <row r="127" ht="17" customHeight="1">
-      <c r="A127" s="46"/>
+      <c r="A127" s="44"/>
       <c r="B127" s="26"/>
       <c r="C127" s="26"/>
       <c r="D127" s="26"/>
@@ -25296,7 +25267,7 @@
       <c r="BI127" s="26"/>
     </row>
     <row r="128" ht="17" customHeight="1">
-      <c r="A128" s="46"/>
+      <c r="A128" s="44"/>
       <c r="B128" s="26"/>
       <c r="C128" s="26"/>
       <c r="D128" s="26"/>
@@ -25359,7 +25330,7 @@
       <c r="BI128" s="26"/>
     </row>
     <row r="129" ht="17" customHeight="1">
-      <c r="A129" s="46"/>
+      <c r="A129" s="44"/>
       <c r="B129" s="26"/>
       <c r="C129" s="26"/>
       <c r="D129" s="26"/>
@@ -25422,7 +25393,7 @@
       <c r="BI129" s="26"/>
     </row>
     <row r="130" ht="17" customHeight="1">
-      <c r="A130" s="46"/>
+      <c r="A130" s="44"/>
       <c r="B130" s="26"/>
       <c r="C130" s="26"/>
       <c r="D130" s="26"/>
@@ -25485,7 +25456,7 @@
       <c r="BI130" s="26"/>
     </row>
     <row r="131" ht="17" customHeight="1">
-      <c r="A131" s="46"/>
+      <c r="A131" s="44"/>
       <c r="B131" s="26"/>
       <c r="C131" s="26"/>
       <c r="D131" s="26"/>
@@ -25548,7 +25519,7 @@
       <c r="BI131" s="26"/>
     </row>
     <row r="132" ht="17" customHeight="1">
-      <c r="A132" s="46"/>
+      <c r="A132" s="44"/>
       <c r="B132" s="26"/>
       <c r="C132" s="26"/>
       <c r="D132" s="26"/>
@@ -25611,7 +25582,7 @@
       <c r="BI132" s="26"/>
     </row>
     <row r="133" ht="17" customHeight="1">
-      <c r="A133" s="46"/>
+      <c r="A133" s="44"/>
       <c r="B133" s="26"/>
       <c r="C133" s="26"/>
       <c r="D133" s="26"/>
@@ -25674,7 +25645,7 @@
       <c r="BI133" s="26"/>
     </row>
     <row r="134" ht="17" customHeight="1">
-      <c r="A134" s="46"/>
+      <c r="A134" s="44"/>
       <c r="B134" s="26"/>
       <c r="C134" s="26"/>
       <c r="D134" s="26"/>
@@ -25737,7 +25708,7 @@
       <c r="BI134" s="26"/>
     </row>
     <row r="135" ht="17" customHeight="1">
-      <c r="A135" s="46"/>
+      <c r="A135" s="44"/>
       <c r="B135" s="26"/>
       <c r="C135" s="26"/>
       <c r="D135" s="26"/>
@@ -25800,7 +25771,7 @@
       <c r="BI135" s="26"/>
     </row>
     <row r="136" ht="17" customHeight="1">
-      <c r="A136" s="46"/>
+      <c r="A136" s="44"/>
       <c r="B136" s="26"/>
       <c r="C136" s="26"/>
       <c r="D136" s="26"/>
@@ -25863,7 +25834,7 @@
       <c r="BI136" s="26"/>
     </row>
     <row r="137" ht="17" customHeight="1">
-      <c r="A137" s="46"/>
+      <c r="A137" s="44"/>
       <c r="B137" s="26"/>
       <c r="C137" s="26"/>
       <c r="D137" s="26"/>
@@ -25926,7 +25897,7 @@
       <c r="BI137" s="26"/>
     </row>
     <row r="138" ht="17" customHeight="1">
-      <c r="A138" s="46"/>
+      <c r="A138" s="44"/>
       <c r="B138" s="26"/>
       <c r="C138" s="26"/>
       <c r="D138" s="26"/>
@@ -25989,7 +25960,7 @@
       <c r="BI138" s="26"/>
     </row>
     <row r="139" ht="17" customHeight="1">
-      <c r="A139" s="46"/>
+      <c r="A139" s="44"/>
       <c r="B139" s="26"/>
       <c r="C139" s="26"/>
       <c r="D139" s="26"/>
@@ -26052,7 +26023,7 @@
       <c r="BI139" s="26"/>
     </row>
     <row r="140" ht="17" customHeight="1">
-      <c r="A140" s="46"/>
+      <c r="A140" s="44"/>
       <c r="B140" s="26"/>
       <c r="C140" s="26"/>
       <c r="D140" s="26"/>
@@ -26115,7 +26086,7 @@
       <c r="BI140" s="26"/>
     </row>
     <row r="141" ht="17" customHeight="1">
-      <c r="A141" s="46"/>
+      <c r="A141" s="44"/>
       <c r="B141" s="26"/>
       <c r="C141" s="26"/>
       <c r="D141" s="26"/>
@@ -26178,7 +26149,7 @@
       <c r="BI141" s="26"/>
     </row>
     <row r="142" ht="17" customHeight="1">
-      <c r="A142" s="46"/>
+      <c r="A142" s="44"/>
       <c r="B142" s="26"/>
       <c r="C142" s="26"/>
       <c r="D142" s="26"/>
@@ -26241,7 +26212,7 @@
       <c r="BI142" s="26"/>
     </row>
     <row r="143" ht="17" customHeight="1">
-      <c r="A143" s="46"/>
+      <c r="A143" s="44"/>
       <c r="B143" s="26"/>
       <c r="C143" s="26"/>
       <c r="D143" s="26"/>
@@ -26304,7 +26275,7 @@
       <c r="BI143" s="26"/>
     </row>
     <row r="144" ht="17" customHeight="1">
-      <c r="A144" s="46"/>
+      <c r="A144" s="44"/>
       <c r="B144" s="26"/>
       <c r="C144" s="26"/>
       <c r="D144" s="26"/>
@@ -26367,7 +26338,7 @@
       <c r="BI144" s="26"/>
     </row>
     <row r="145" ht="17" customHeight="1">
-      <c r="A145" s="46"/>
+      <c r="A145" s="44"/>
       <c r="B145" s="26"/>
       <c r="C145" s="26"/>
       <c r="D145" s="26"/>
@@ -26430,7 +26401,7 @@
       <c r="BI145" s="26"/>
     </row>
     <row r="146" ht="17" customHeight="1">
-      <c r="A146" s="46"/>
+      <c r="A146" s="44"/>
       <c r="B146" s="26"/>
       <c r="C146" s="26"/>
       <c r="D146" s="26"/>
@@ -26493,7 +26464,7 @@
       <c r="BI146" s="26"/>
     </row>
     <row r="147" ht="17" customHeight="1">
-      <c r="A147" s="46"/>
+      <c r="A147" s="44"/>
       <c r="B147" s="26"/>
       <c r="C147" s="26"/>
       <c r="D147" s="26"/>
@@ -26556,7 +26527,7 @@
       <c r="BI147" s="26"/>
     </row>
     <row r="148" ht="17" customHeight="1">
-      <c r="A148" s="46"/>
+      <c r="A148" s="44"/>
       <c r="B148" s="26"/>
       <c r="C148" s="26"/>
       <c r="D148" s="26"/>
@@ -26619,7 +26590,7 @@
       <c r="BI148" s="26"/>
     </row>
     <row r="149" ht="17" customHeight="1">
-      <c r="A149" s="46"/>
+      <c r="A149" s="44"/>
       <c r="B149" s="26"/>
       <c r="C149" s="26"/>
       <c r="D149" s="26"/>
@@ -26682,7 +26653,7 @@
       <c r="BI149" s="26"/>
     </row>
     <row r="150" ht="17" customHeight="1">
-      <c r="A150" s="46"/>
+      <c r="A150" s="44"/>
       <c r="B150" s="26"/>
       <c r="C150" s="26"/>
       <c r="D150" s="26"/>
@@ -26745,7 +26716,7 @@
       <c r="BI150" s="26"/>
     </row>
     <row r="151" ht="17" customHeight="1">
-      <c r="A151" s="46"/>
+      <c r="A151" s="44"/>
       <c r="B151" s="26"/>
       <c r="C151" s="26"/>
       <c r="D151" s="26"/>
@@ -26808,7 +26779,7 @@
       <c r="BI151" s="26"/>
     </row>
     <row r="152" ht="17" customHeight="1">
-      <c r="A152" s="46"/>
+      <c r="A152" s="44"/>
       <c r="B152" s="26"/>
       <c r="C152" s="26"/>
       <c r="D152" s="26"/>
@@ -26871,7 +26842,7 @@
       <c r="BI152" s="26"/>
     </row>
     <row r="153" ht="17" customHeight="1">
-      <c r="A153" s="46"/>
+      <c r="A153" s="44"/>
       <c r="B153" s="26"/>
       <c r="C153" s="26"/>
       <c r="D153" s="26"/>
@@ -26934,7 +26905,7 @@
       <c r="BI153" s="26"/>
     </row>
     <row r="154" ht="17" customHeight="1">
-      <c r="A154" s="46"/>
+      <c r="A154" s="44"/>
       <c r="B154" s="26"/>
       <c r="C154" s="26"/>
       <c r="D154" s="26"/>
@@ -26997,7 +26968,7 @@
       <c r="BI154" s="26"/>
     </row>
     <row r="155" ht="17" customHeight="1">
-      <c r="A155" s="46"/>
+      <c r="A155" s="44"/>
       <c r="B155" s="26"/>
       <c r="C155" s="26"/>
       <c r="D155" s="26"/>
@@ -27060,7 +27031,7 @@
       <c r="BI155" s="26"/>
     </row>
     <row r="156" ht="17" customHeight="1">
-      <c r="A156" s="46"/>
+      <c r="A156" s="44"/>
       <c r="B156" s="26"/>
       <c r="C156" s="26"/>
       <c r="D156" s="26"/>
@@ -27123,7 +27094,7 @@
       <c r="BI156" s="26"/>
     </row>
     <row r="157" ht="17" customHeight="1">
-      <c r="A157" s="46"/>
+      <c r="A157" s="44"/>
       <c r="B157" s="26"/>
       <c r="C157" s="26"/>
       <c r="D157" s="26"/>
@@ -27186,7 +27157,7 @@
       <c r="BI157" s="26"/>
     </row>
     <row r="158" ht="17" customHeight="1">
-      <c r="A158" s="46"/>
+      <c r="A158" s="44"/>
       <c r="B158" s="26"/>
       <c r="C158" s="26"/>
       <c r="D158" s="26"/>
@@ -27249,7 +27220,7 @@
       <c r="BI158" s="26"/>
     </row>
     <row r="159" ht="17" customHeight="1">
-      <c r="A159" s="46"/>
+      <c r="A159" s="44"/>
       <c r="B159" s="26"/>
       <c r="C159" s="26"/>
       <c r="D159" s="26"/>
@@ -27312,7 +27283,7 @@
       <c r="BI159" s="26"/>
     </row>
     <row r="160" ht="17" customHeight="1">
-      <c r="A160" s="46"/>
+      <c r="A160" s="44"/>
       <c r="B160" s="26"/>
       <c r="C160" s="26"/>
       <c r="D160" s="26"/>
@@ -27375,7 +27346,7 @@
       <c r="BI160" s="26"/>
     </row>
     <row r="161" ht="17" customHeight="1">
-      <c r="A161" s="46"/>
+      <c r="A161" s="44"/>
       <c r="B161" s="26"/>
       <c r="C161" s="26"/>
       <c r="D161" s="26"/>
@@ -27438,7 +27409,7 @@
       <c r="BI161" s="26"/>
     </row>
     <row r="162" ht="17" customHeight="1">
-      <c r="A162" s="46"/>
+      <c r="A162" s="44"/>
       <c r="B162" s="26"/>
       <c r="C162" s="26"/>
       <c r="D162" s="26"/>
@@ -27501,7 +27472,7 @@
       <c r="BI162" s="26"/>
     </row>
     <row r="163" ht="17" customHeight="1">
-      <c r="A163" s="46"/>
+      <c r="A163" s="44"/>
       <c r="B163" s="26"/>
       <c r="C163" s="26"/>
       <c r="D163" s="26"/>
@@ -27564,7 +27535,7 @@
       <c r="BI163" s="26"/>
     </row>
     <row r="164" ht="17" customHeight="1">
-      <c r="A164" s="46"/>
+      <c r="A164" s="44"/>
       <c r="B164" s="26"/>
       <c r="C164" s="26"/>
       <c r="D164" s="26"/>
@@ -27627,7 +27598,7 @@
       <c r="BI164" s="26"/>
     </row>
     <row r="165" ht="17" customHeight="1">
-      <c r="A165" s="46"/>
+      <c r="A165" s="44"/>
       <c r="B165" s="26"/>
       <c r="C165" s="26"/>
       <c r="D165" s="26"/>
@@ -27690,7 +27661,7 @@
       <c r="BI165" s="26"/>
     </row>
     <row r="166" ht="17" customHeight="1">
-      <c r="A166" s="46"/>
+      <c r="A166" s="44"/>
       <c r="B166" s="26"/>
       <c r="C166" s="26"/>
       <c r="D166" s="26"/>
@@ -27753,7 +27724,7 @@
       <c r="BI166" s="26"/>
     </row>
     <row r="167" ht="17" customHeight="1">
-      <c r="A167" s="46"/>
+      <c r="A167" s="44"/>
       <c r="B167" s="26"/>
       <c r="C167" s="26"/>
       <c r="D167" s="26"/>
@@ -27816,7 +27787,7 @@
       <c r="BI167" s="26"/>
     </row>
     <row r="168" ht="17" customHeight="1">
-      <c r="A168" s="46"/>
+      <c r="A168" s="44"/>
       <c r="B168" s="26"/>
       <c r="C168" s="26"/>
       <c r="D168" s="26"/>
@@ -27879,7 +27850,7 @@
       <c r="BI168" s="26"/>
     </row>
     <row r="169" ht="17" customHeight="1">
-      <c r="A169" s="46"/>
+      <c r="A169" s="44"/>
       <c r="B169" s="26"/>
       <c r="C169" s="26"/>
       <c r="D169" s="26"/>
@@ -27942,7 +27913,7 @@
       <c r="BI169" s="26"/>
     </row>
     <row r="170" ht="17" customHeight="1">
-      <c r="A170" s="46"/>
+      <c r="A170" s="44"/>
       <c r="B170" s="26"/>
       <c r="C170" s="26"/>
       <c r="D170" s="26"/>
@@ -28005,7 +27976,7 @@
       <c r="BI170" s="26"/>
     </row>
     <row r="171" ht="17" customHeight="1">
-      <c r="A171" s="46"/>
+      <c r="A171" s="44"/>
       <c r="B171" s="26"/>
       <c r="C171" s="26"/>
       <c r="D171" s="26"/>
@@ -28068,7 +28039,7 @@
       <c r="BI171" s="26"/>
     </row>
     <row r="172" ht="17" customHeight="1">
-      <c r="A172" s="46"/>
+      <c r="A172" s="44"/>
       <c r="B172" s="26"/>
       <c r="C172" s="26"/>
       <c r="D172" s="26"/>
@@ -28131,7 +28102,7 @@
       <c r="BI172" s="26"/>
     </row>
     <row r="173" ht="17" customHeight="1">
-      <c r="A173" s="46"/>
+      <c r="A173" s="44"/>
       <c r="B173" s="26"/>
       <c r="C173" s="26"/>
       <c r="D173" s="26"/>
@@ -28194,7 +28165,7 @@
       <c r="BI173" s="26"/>
     </row>
     <row r="174" ht="17" customHeight="1">
-      <c r="A174" s="46"/>
+      <c r="A174" s="44"/>
       <c r="B174" s="26"/>
       <c r="C174" s="26"/>
       <c r="D174" s="26"/>
@@ -28257,7 +28228,7 @@
       <c r="BI174" s="26"/>
     </row>
     <row r="175" ht="17" customHeight="1">
-      <c r="A175" s="46"/>
+      <c r="A175" s="44"/>
       <c r="B175" s="26"/>
       <c r="C175" s="26"/>
       <c r="D175" s="26"/>
@@ -28320,7 +28291,7 @@
       <c r="BI175" s="26"/>
     </row>
     <row r="176" ht="17" customHeight="1">
-      <c r="A176" s="46"/>
+      <c r="A176" s="44"/>
       <c r="B176" s="26"/>
       <c r="C176" s="26"/>
       <c r="D176" s="26"/>
@@ -28383,7 +28354,7 @@
       <c r="BI176" s="26"/>
     </row>
     <row r="177" ht="17" customHeight="1">
-      <c r="A177" s="46"/>
+      <c r="A177" s="44"/>
       <c r="B177" s="26"/>
       <c r="C177" s="26"/>
       <c r="D177" s="26"/>
@@ -28446,7 +28417,7 @@
       <c r="BI177" s="26"/>
     </row>
     <row r="178" ht="17" customHeight="1">
-      <c r="A178" s="46"/>
+      <c r="A178" s="44"/>
       <c r="B178" s="26"/>
       <c r="C178" s="26"/>
       <c r="D178" s="26"/>
@@ -28509,7 +28480,7 @@
       <c r="BI178" s="26"/>
     </row>
     <row r="179" ht="17" customHeight="1">
-      <c r="A179" s="46"/>
+      <c r="A179" s="44"/>
       <c r="B179" s="26"/>
       <c r="C179" s="26"/>
       <c r="D179" s="26"/>
@@ -28572,7 +28543,7 @@
       <c r="BI179" s="26"/>
     </row>
     <row r="180" ht="17" customHeight="1">
-      <c r="A180" s="46"/>
+      <c r="A180" s="44"/>
       <c r="B180" s="26"/>
       <c r="C180" s="26"/>
       <c r="D180" s="26"/>
@@ -28635,7 +28606,7 @@
       <c r="BI180" s="26"/>
     </row>
     <row r="181" ht="17" customHeight="1">
-      <c r="A181" s="46"/>
+      <c r="A181" s="44"/>
       <c r="B181" s="26"/>
       <c r="C181" s="26"/>
       <c r="D181" s="26"/>
@@ -28698,7 +28669,7 @@
       <c r="BI181" s="26"/>
     </row>
     <row r="182" ht="17" customHeight="1">
-      <c r="A182" s="46"/>
+      <c r="A182" s="44"/>
       <c r="B182" s="26"/>
       <c r="C182" s="26"/>
       <c r="D182" s="26"/>
@@ -28761,7 +28732,7 @@
       <c r="BI182" s="26"/>
     </row>
     <row r="183" ht="17" customHeight="1">
-      <c r="A183" s="46"/>
+      <c r="A183" s="44"/>
       <c r="B183" s="26"/>
       <c r="C183" s="26"/>
       <c r="D183" s="26"/>
@@ -28824,7 +28795,7 @@
       <c r="BI183" s="26"/>
     </row>
     <row r="184" ht="17" customHeight="1">
-      <c r="A184" s="46"/>
+      <c r="A184" s="44"/>
       <c r="B184" s="26"/>
       <c r="C184" s="26"/>
       <c r="D184" s="26"/>
@@ -28887,7 +28858,7 @@
       <c r="BI184" s="26"/>
     </row>
     <row r="185" ht="17" customHeight="1">
-      <c r="A185" s="46"/>
+      <c r="A185" s="44"/>
       <c r="B185" s="26"/>
       <c r="C185" s="26"/>
       <c r="D185" s="26"/>
@@ -28950,7 +28921,7 @@
       <c r="BI185" s="26"/>
     </row>
     <row r="186" ht="17" customHeight="1">
-      <c r="A186" s="46"/>
+      <c r="A186" s="44"/>
       <c r="B186" s="26"/>
       <c r="C186" s="26"/>
       <c r="D186" s="26"/>
@@ -29013,7 +28984,7 @@
       <c r="BI186" s="26"/>
     </row>
     <row r="187" ht="17" customHeight="1">
-      <c r="A187" s="46"/>
+      <c r="A187" s="44"/>
       <c r="B187" s="26"/>
       <c r="C187" s="26"/>
       <c r="D187" s="26"/>
@@ -29076,7 +29047,7 @@
       <c r="BI187" s="26"/>
     </row>
     <row r="188" ht="17" customHeight="1">
-      <c r="A188" s="46"/>
+      <c r="A188" s="44"/>
       <c r="B188" s="26"/>
       <c r="C188" s="26"/>
       <c r="D188" s="26"/>
@@ -29139,7 +29110,7 @@
       <c r="BI188" s="26"/>
     </row>
     <row r="189" ht="17" customHeight="1">
-      <c r="A189" s="46"/>
+      <c r="A189" s="44"/>
       <c r="B189" s="26"/>
       <c r="C189" s="26"/>
       <c r="D189" s="26"/>
@@ -29202,7 +29173,7 @@
       <c r="BI189" s="26"/>
     </row>
     <row r="190" ht="17" customHeight="1">
-      <c r="A190" s="46"/>
+      <c r="A190" s="44"/>
       <c r="B190" s="26"/>
       <c r="C190" s="26"/>
       <c r="D190" s="26"/>
@@ -29265,7 +29236,7 @@
       <c r="BI190" s="26"/>
     </row>
     <row r="191" ht="17" customHeight="1">
-      <c r="A191" s="46"/>
+      <c r="A191" s="44"/>
       <c r="B191" s="26"/>
       <c r="C191" s="26"/>
       <c r="D191" s="26"/>
@@ -29328,7 +29299,7 @@
       <c r="BI191" s="26"/>
     </row>
     <row r="192" ht="17" customHeight="1">
-      <c r="A192" s="46"/>
+      <c r="A192" s="44"/>
       <c r="B192" s="26"/>
       <c r="C192" s="26"/>
       <c r="D192" s="26"/>
@@ -29391,7 +29362,7 @@
       <c r="BI192" s="26"/>
     </row>
     <row r="193" ht="17" customHeight="1">
-      <c r="A193" s="46"/>
+      <c r="A193" s="44"/>
       <c r="B193" s="26"/>
       <c r="C193" s="26"/>
       <c r="D193" s="26"/>
@@ -29454,7 +29425,7 @@
       <c r="BI193" s="26"/>
     </row>
     <row r="194" ht="17" customHeight="1">
-      <c r="A194" s="46"/>
+      <c r="A194" s="44"/>
       <c r="B194" s="26"/>
       <c r="C194" s="26"/>
       <c r="D194" s="26"/>
@@ -29517,7 +29488,7 @@
       <c r="BI194" s="26"/>
     </row>
     <row r="195" ht="17" customHeight="1">
-      <c r="A195" s="46"/>
+      <c r="A195" s="44"/>
       <c r="B195" s="26"/>
       <c r="C195" s="26"/>
       <c r="D195" s="26"/>
@@ -29598,83 +29569,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="54" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="54" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="54" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="54" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="54" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="54" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="51" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="51" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="51" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="51" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="51" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="55"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="55"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.787402" right="0.787402" top="0.984252" bottom="0.984252" header="0.492126" footer="0.492126"/>
@@ -29693,83 +29664,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="56" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="56" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="56" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="56" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="56" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="56" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="53" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="53" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="53" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="53" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="53" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="55"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="55"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.787402" right="0.787402" top="0.984252" bottom="0.984252" header="0.492126" footer="0.492126"/>

</xml_diff>